<commit_message>
Modified loss models to reflect dissolution of Dutch Antilles and Sudan, Making use of new LocalTime class in impactutils, handling scenarios, renamed pageradmin to adminpager for tab completion purposes.
</commit_message>
<xml_diff>
--- a/losspager/data/countries.xlsx
+++ b/losspager/data/countries.xlsx
@@ -557,9 +557,6 @@
     <t>CRI</t>
   </si>
   <si>
-    <t>C√¥te d'Ivoire</t>
-  </si>
-  <si>
     <t>CI</t>
   </si>
   <si>
@@ -584,9 +581,6 @@
     <t>CUB</t>
   </si>
   <si>
-    <t>Cura√ßao</t>
-  </si>
-  <si>
     <t>CW</t>
   </si>
   <si>
@@ -1754,9 +1748,6 @@
     <t>RWA</t>
   </si>
   <si>
-    <t>Saint Barth√©lemy</t>
-  </si>
-  <si>
     <t>BL</t>
   </si>
   <si>
@@ -2394,6 +2385,15 @@
   </si>
   <si>
     <t>UKN</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Saint Barthelemy</t>
   </si>
 </sst>
 </file>
@@ -2856,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3822,13 +3822,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
+        <v>782</v>
+      </c>
+      <c r="B56" t="s">
         <v>172</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>173</v>
-      </c>
-      <c r="C56" t="s">
-        <v>174</v>
       </c>
       <c r="D56">
         <v>384</v>
@@ -3839,13 +3839,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57" t="s">
         <v>175</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>176</v>
-      </c>
-      <c r="C57" t="s">
-        <v>177</v>
       </c>
       <c r="D57">
         <v>191</v>
@@ -3856,13 +3856,13 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" t="s">
         <v>178</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>179</v>
-      </c>
-      <c r="C58" t="s">
-        <v>180</v>
       </c>
       <c r="D58">
         <v>192</v>
@@ -3873,13 +3873,13 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
+        <v>783</v>
+      </c>
+      <c r="B59" t="s">
+        <v>180</v>
+      </c>
+      <c r="C59" t="s">
         <v>181</v>
-      </c>
-      <c r="B59" t="s">
-        <v>182</v>
-      </c>
-      <c r="C59" t="s">
-        <v>183</v>
       </c>
       <c r="D59">
         <v>531</v>
@@ -3890,13 +3890,13 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" t="s">
         <v>184</v>
-      </c>
-      <c r="B60" t="s">
-        <v>185</v>
-      </c>
-      <c r="C60" t="s">
-        <v>186</v>
       </c>
       <c r="D60">
         <v>196</v>
@@ -3907,13 +3907,13 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" t="s">
         <v>187</v>
-      </c>
-      <c r="B61" t="s">
-        <v>188</v>
-      </c>
-      <c r="C61" t="s">
-        <v>189</v>
       </c>
       <c r="D61">
         <v>203</v>
@@ -3924,13 +3924,13 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" t="s">
+        <v>189</v>
+      </c>
+      <c r="C62" t="s">
         <v>190</v>
-      </c>
-      <c r="B62" t="s">
-        <v>191</v>
-      </c>
-      <c r="C62" t="s">
-        <v>192</v>
       </c>
       <c r="D62">
         <v>208</v>
@@ -3941,13 +3941,13 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" t="s">
         <v>193</v>
-      </c>
-      <c r="B63" t="s">
-        <v>194</v>
-      </c>
-      <c r="C63" t="s">
-        <v>195</v>
       </c>
       <c r="D63">
         <v>262</v>
@@ -3958,13 +3958,13 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" t="s">
         <v>196</v>
-      </c>
-      <c r="B64" t="s">
-        <v>197</v>
-      </c>
-      <c r="C64" t="s">
-        <v>198</v>
       </c>
       <c r="D64">
         <v>212</v>
@@ -3975,13 +3975,13 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" t="s">
         <v>199</v>
-      </c>
-      <c r="B65" t="s">
-        <v>200</v>
-      </c>
-      <c r="C65" t="s">
-        <v>201</v>
       </c>
       <c r="D65">
         <v>214</v>
@@ -3992,13 +3992,13 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" t="s">
         <v>202</v>
-      </c>
-      <c r="B66" t="s">
-        <v>203</v>
-      </c>
-      <c r="C66" t="s">
-        <v>204</v>
       </c>
       <c r="D66">
         <v>218</v>
@@ -4009,13 +4009,13 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" t="s">
         <v>205</v>
-      </c>
-      <c r="B67" t="s">
-        <v>206</v>
-      </c>
-      <c r="C67" t="s">
-        <v>207</v>
       </c>
       <c r="D67">
         <v>818</v>
@@ -4026,13 +4026,13 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" t="s">
         <v>208</v>
-      </c>
-      <c r="B68" t="s">
-        <v>209</v>
-      </c>
-      <c r="C68" t="s">
-        <v>210</v>
       </c>
       <c r="D68">
         <v>222</v>
@@ -4043,13 +4043,13 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
+        <v>209</v>
+      </c>
+      <c r="B69" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" t="s">
         <v>211</v>
-      </c>
-      <c r="B69" t="s">
-        <v>212</v>
-      </c>
-      <c r="C69" t="s">
-        <v>213</v>
       </c>
       <c r="D69">
         <v>226</v>
@@ -4060,13 +4060,13 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" t="s">
         <v>214</v>
-      </c>
-      <c r="B70" t="s">
-        <v>215</v>
-      </c>
-      <c r="C70" t="s">
-        <v>216</v>
       </c>
       <c r="D70">
         <v>232</v>
@@ -4077,13 +4077,13 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" t="s">
         <v>217</v>
-      </c>
-      <c r="B71" t="s">
-        <v>218</v>
-      </c>
-      <c r="C71" t="s">
-        <v>219</v>
       </c>
       <c r="D71">
         <v>233</v>
@@ -4094,13 +4094,13 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" t="s">
+        <v>219</v>
+      </c>
+      <c r="C72" t="s">
         <v>220</v>
-      </c>
-      <c r="B72" t="s">
-        <v>221</v>
-      </c>
-      <c r="C72" t="s">
-        <v>222</v>
       </c>
       <c r="D72">
         <v>231</v>
@@ -4111,13 +4111,13 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
+        <v>221</v>
+      </c>
+      <c r="B73" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" t="s">
         <v>223</v>
-      </c>
-      <c r="B73" t="s">
-        <v>224</v>
-      </c>
-      <c r="C73" t="s">
-        <v>225</v>
       </c>
       <c r="D73">
         <v>238</v>
@@ -4128,13 +4128,13 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" t="s">
         <v>226</v>
-      </c>
-      <c r="B74" t="s">
-        <v>227</v>
-      </c>
-      <c r="C74" t="s">
-        <v>228</v>
       </c>
       <c r="D74">
         <v>234</v>
@@ -4145,13 +4145,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
+        <v>227</v>
+      </c>
+      <c r="B75" t="s">
+        <v>228</v>
+      </c>
+      <c r="C75" t="s">
         <v>229</v>
-      </c>
-      <c r="B75" t="s">
-        <v>230</v>
-      </c>
-      <c r="C75" t="s">
-        <v>231</v>
       </c>
       <c r="D75">
         <v>242</v>
@@ -4162,13 +4162,13 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" t="s">
         <v>232</v>
-      </c>
-      <c r="B76" t="s">
-        <v>233</v>
-      </c>
-      <c r="C76" t="s">
-        <v>234</v>
       </c>
       <c r="D76">
         <v>246</v>
@@ -4179,13 +4179,13 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
+        <v>233</v>
+      </c>
+      <c r="B77" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" t="s">
         <v>235</v>
-      </c>
-      <c r="B77" t="s">
-        <v>236</v>
-      </c>
-      <c r="C77" t="s">
-        <v>237</v>
       </c>
       <c r="D77">
         <v>250</v>
@@ -4196,13 +4196,13 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
+        <v>236</v>
+      </c>
+      <c r="B78" t="s">
+        <v>237</v>
+      </c>
+      <c r="C78" t="s">
         <v>238</v>
-      </c>
-      <c r="B78" t="s">
-        <v>239</v>
-      </c>
-      <c r="C78" t="s">
-        <v>240</v>
       </c>
       <c r="D78">
         <v>254</v>
@@ -4213,13 +4213,13 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
+        <v>239</v>
+      </c>
+      <c r="B79" t="s">
+        <v>240</v>
+      </c>
+      <c r="C79" t="s">
         <v>241</v>
-      </c>
-      <c r="B79" t="s">
-        <v>242</v>
-      </c>
-      <c r="C79" t="s">
-        <v>243</v>
       </c>
       <c r="D79">
         <v>258</v>
@@ -4230,13 +4230,13 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
+        <v>242</v>
+      </c>
+      <c r="B80" t="s">
+        <v>243</v>
+      </c>
+      <c r="C80" t="s">
         <v>244</v>
-      </c>
-      <c r="B80" t="s">
-        <v>245</v>
-      </c>
-      <c r="C80" t="s">
-        <v>246</v>
       </c>
       <c r="D80">
         <v>260</v>
@@ -4247,13 +4247,13 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
+        <v>245</v>
+      </c>
+      <c r="B81" t="s">
+        <v>246</v>
+      </c>
+      <c r="C81" t="s">
         <v>247</v>
-      </c>
-      <c r="B81" t="s">
-        <v>248</v>
-      </c>
-      <c r="C81" t="s">
-        <v>249</v>
       </c>
       <c r="D81">
         <v>266</v>
@@ -4264,13 +4264,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
+        <v>248</v>
+      </c>
+      <c r="B82" t="s">
+        <v>249</v>
+      </c>
+      <c r="C82" t="s">
         <v>250</v>
-      </c>
-      <c r="B82" t="s">
-        <v>251</v>
-      </c>
-      <c r="C82" t="s">
-        <v>252</v>
       </c>
       <c r="D82">
         <v>270</v>
@@ -4281,13 +4281,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
+        <v>251</v>
+      </c>
+      <c r="B83" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" t="s">
         <v>253</v>
-      </c>
-      <c r="B83" t="s">
-        <v>254</v>
-      </c>
-      <c r="C83" t="s">
-        <v>255</v>
       </c>
       <c r="D83">
         <v>268</v>
@@ -4298,13 +4298,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" t="s">
+        <v>255</v>
+      </c>
+      <c r="C84" t="s">
         <v>256</v>
-      </c>
-      <c r="B84" t="s">
-        <v>257</v>
-      </c>
-      <c r="C84" t="s">
-        <v>258</v>
       </c>
       <c r="D84">
         <v>276</v>
@@ -4315,13 +4315,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
+        <v>257</v>
+      </c>
+      <c r="B85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C85" t="s">
         <v>259</v>
-      </c>
-      <c r="B85" t="s">
-        <v>260</v>
-      </c>
-      <c r="C85" t="s">
-        <v>261</v>
       </c>
       <c r="D85">
         <v>288</v>
@@ -4332,13 +4332,13 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
+        <v>260</v>
+      </c>
+      <c r="B86" t="s">
+        <v>261</v>
+      </c>
+      <c r="C86" t="s">
         <v>262</v>
-      </c>
-      <c r="B86" t="s">
-        <v>263</v>
-      </c>
-      <c r="C86" t="s">
-        <v>264</v>
       </c>
       <c r="D86">
         <v>292</v>
@@ -4349,13 +4349,13 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
+        <v>263</v>
+      </c>
+      <c r="B87" t="s">
+        <v>264</v>
+      </c>
+      <c r="C87" t="s">
         <v>265</v>
-      </c>
-      <c r="B87" t="s">
-        <v>266</v>
-      </c>
-      <c r="C87" t="s">
-        <v>267</v>
       </c>
       <c r="D87">
         <v>300</v>
@@ -4366,13 +4366,13 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
+        <v>266</v>
+      </c>
+      <c r="B88" t="s">
+        <v>267</v>
+      </c>
+      <c r="C88" t="s">
         <v>268</v>
-      </c>
-      <c r="B88" t="s">
-        <v>269</v>
-      </c>
-      <c r="C88" t="s">
-        <v>270</v>
       </c>
       <c r="D88">
         <v>304</v>
@@ -4383,13 +4383,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
+        <v>269</v>
+      </c>
+      <c r="B89" t="s">
+        <v>270</v>
+      </c>
+      <c r="C89" t="s">
         <v>271</v>
-      </c>
-      <c r="B89" t="s">
-        <v>272</v>
-      </c>
-      <c r="C89" t="s">
-        <v>273</v>
       </c>
       <c r="D89">
         <v>308</v>
@@ -4400,13 +4400,13 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
+        <v>272</v>
+      </c>
+      <c r="B90" t="s">
+        <v>273</v>
+      </c>
+      <c r="C90" t="s">
         <v>274</v>
-      </c>
-      <c r="B90" t="s">
-        <v>275</v>
-      </c>
-      <c r="C90" t="s">
-        <v>276</v>
       </c>
       <c r="D90">
         <v>312</v>
@@ -4417,13 +4417,13 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
+        <v>275</v>
+      </c>
+      <c r="B91" t="s">
+        <v>276</v>
+      </c>
+      <c r="C91" t="s">
         <v>277</v>
-      </c>
-      <c r="B91" t="s">
-        <v>278</v>
-      </c>
-      <c r="C91" t="s">
-        <v>279</v>
       </c>
       <c r="D91">
         <v>316</v>
@@ -4434,13 +4434,13 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
+        <v>278</v>
+      </c>
+      <c r="B92" t="s">
+        <v>279</v>
+      </c>
+      <c r="C92" t="s">
         <v>280</v>
-      </c>
-      <c r="B92" t="s">
-        <v>281</v>
-      </c>
-      <c r="C92" t="s">
-        <v>282</v>
       </c>
       <c r="D92">
         <v>320</v>
@@ -4451,13 +4451,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
+        <v>281</v>
+      </c>
+      <c r="B93" t="s">
+        <v>282</v>
+      </c>
+      <c r="C93" t="s">
         <v>283</v>
-      </c>
-      <c r="B93" t="s">
-        <v>284</v>
-      </c>
-      <c r="C93" t="s">
-        <v>285</v>
       </c>
       <c r="D93">
         <v>831</v>
@@ -4468,13 +4468,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
+        <v>284</v>
+      </c>
+      <c r="B94" t="s">
+        <v>285</v>
+      </c>
+      <c r="C94" t="s">
         <v>286</v>
-      </c>
-      <c r="B94" t="s">
-        <v>287</v>
-      </c>
-      <c r="C94" t="s">
-        <v>288</v>
       </c>
       <c r="D94">
         <v>324</v>
@@ -4485,13 +4485,13 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
+        <v>287</v>
+      </c>
+      <c r="B95" t="s">
+        <v>288</v>
+      </c>
+      <c r="C95" t="s">
         <v>289</v>
-      </c>
-      <c r="B95" t="s">
-        <v>290</v>
-      </c>
-      <c r="C95" t="s">
-        <v>291</v>
       </c>
       <c r="D95">
         <v>624</v>
@@ -4502,13 +4502,13 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
+        <v>290</v>
+      </c>
+      <c r="B96" t="s">
+        <v>291</v>
+      </c>
+      <c r="C96" t="s">
         <v>292</v>
-      </c>
-      <c r="B96" t="s">
-        <v>293</v>
-      </c>
-      <c r="C96" t="s">
-        <v>294</v>
       </c>
       <c r="D96">
         <v>328</v>
@@ -4519,13 +4519,13 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
+        <v>293</v>
+      </c>
+      <c r="B97" t="s">
+        <v>294</v>
+      </c>
+      <c r="C97" t="s">
         <v>295</v>
-      </c>
-      <c r="B97" t="s">
-        <v>296</v>
-      </c>
-      <c r="C97" t="s">
-        <v>297</v>
       </c>
       <c r="D97">
         <v>332</v>
@@ -4536,13 +4536,13 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
+        <v>296</v>
+      </c>
+      <c r="B98" t="s">
+        <v>297</v>
+      </c>
+      <c r="C98" t="s">
         <v>298</v>
-      </c>
-      <c r="B98" t="s">
-        <v>299</v>
-      </c>
-      <c r="C98" t="s">
-        <v>300</v>
       </c>
       <c r="D98">
         <v>334</v>
@@ -4553,19 +4553,19 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
+        <v>299</v>
+      </c>
+      <c r="B99" t="s">
+        <v>300</v>
+      </c>
+      <c r="C99" t="s">
         <v>301</v>
-      </c>
-      <c r="B99" t="s">
-        <v>302</v>
-      </c>
-      <c r="C99" t="s">
-        <v>303</v>
       </c>
       <c r="D99">
         <v>336</v>
       </c>
       <c r="E99" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F99" s="2">
         <v>842</v>
@@ -4573,13 +4573,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
+        <v>303</v>
+      </c>
+      <c r="B100" t="s">
+        <v>304</v>
+      </c>
+      <c r="C100" t="s">
         <v>305</v>
-      </c>
-      <c r="B100" t="s">
-        <v>306</v>
-      </c>
-      <c r="C100" t="s">
-        <v>307</v>
       </c>
       <c r="D100">
         <v>340</v>
@@ -4590,13 +4590,13 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
+        <v>306</v>
+      </c>
+      <c r="B101" t="s">
+        <v>307</v>
+      </c>
+      <c r="C101" t="s">
         <v>308</v>
-      </c>
-      <c r="B101" t="s">
-        <v>309</v>
-      </c>
-      <c r="C101" t="s">
-        <v>310</v>
       </c>
       <c r="D101">
         <v>344</v>
@@ -4607,13 +4607,13 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
+        <v>309</v>
+      </c>
+      <c r="B102" t="s">
+        <v>310</v>
+      </c>
+      <c r="C102" t="s">
         <v>311</v>
-      </c>
-      <c r="B102" t="s">
-        <v>312</v>
-      </c>
-      <c r="C102" t="s">
-        <v>313</v>
       </c>
       <c r="D102">
         <v>348</v>
@@ -4624,13 +4624,13 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
+        <v>312</v>
+      </c>
+      <c r="B103" t="s">
+        <v>313</v>
+      </c>
+      <c r="C103" t="s">
         <v>314</v>
-      </c>
-      <c r="B103" t="s">
-        <v>315</v>
-      </c>
-      <c r="C103" t="s">
-        <v>316</v>
       </c>
       <c r="D103">
         <v>352</v>
@@ -4641,13 +4641,13 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
+        <v>315</v>
+      </c>
+      <c r="B104" t="s">
+        <v>316</v>
+      </c>
+      <c r="C104" t="s">
         <v>317</v>
-      </c>
-      <c r="B104" t="s">
-        <v>318</v>
-      </c>
-      <c r="C104" t="s">
-        <v>319</v>
       </c>
       <c r="D104">
         <v>356</v>
@@ -4658,13 +4658,13 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
+        <v>318</v>
+      </c>
+      <c r="B105" t="s">
+        <v>319</v>
+      </c>
+      <c r="C105" t="s">
         <v>320</v>
-      </c>
-      <c r="B105" t="s">
-        <v>321</v>
-      </c>
-      <c r="C105" t="s">
-        <v>322</v>
       </c>
       <c r="D105">
         <v>360</v>
@@ -4675,19 +4675,19 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
+        <v>321</v>
+      </c>
+      <c r="B106" t="s">
+        <v>322</v>
+      </c>
+      <c r="C106" t="s">
         <v>323</v>
-      </c>
-      <c r="B106" t="s">
-        <v>324</v>
-      </c>
-      <c r="C106" t="s">
-        <v>325</v>
       </c>
       <c r="D106">
         <v>364</v>
       </c>
       <c r="E106" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F106" s="2">
         <v>79546600</v>
@@ -4695,13 +4695,13 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
+        <v>325</v>
+      </c>
+      <c r="B107" t="s">
+        <v>326</v>
+      </c>
+      <c r="C107" t="s">
         <v>327</v>
-      </c>
-      <c r="B107" t="s">
-        <v>328</v>
-      </c>
-      <c r="C107" t="s">
-        <v>329</v>
       </c>
       <c r="D107">
         <v>368</v>
@@ -4712,13 +4712,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
+        <v>328</v>
+      </c>
+      <c r="B108" t="s">
+        <v>329</v>
+      </c>
+      <c r="C108" t="s">
         <v>330</v>
-      </c>
-      <c r="B108" t="s">
-        <v>331</v>
-      </c>
-      <c r="C108" t="s">
-        <v>332</v>
       </c>
       <c r="D108">
         <v>372</v>
@@ -4729,13 +4729,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
+        <v>331</v>
+      </c>
+      <c r="B109" t="s">
+        <v>332</v>
+      </c>
+      <c r="C109" t="s">
         <v>333</v>
-      </c>
-      <c r="B109" t="s">
-        <v>334</v>
-      </c>
-      <c r="C109" t="s">
-        <v>335</v>
       </c>
       <c r="D109">
         <v>833</v>
@@ -4746,13 +4746,13 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
+        <v>334</v>
+      </c>
+      <c r="B110" t="s">
+        <v>335</v>
+      </c>
+      <c r="C110" t="s">
         <v>336</v>
-      </c>
-      <c r="B110" t="s">
-        <v>337</v>
-      </c>
-      <c r="C110" t="s">
-        <v>338</v>
       </c>
       <c r="D110">
         <v>376</v>
@@ -4763,13 +4763,13 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
+        <v>337</v>
+      </c>
+      <c r="B111" t="s">
+        <v>338</v>
+      </c>
+      <c r="C111" t="s">
         <v>339</v>
-      </c>
-      <c r="B111" t="s">
-        <v>340</v>
-      </c>
-      <c r="C111" t="s">
-        <v>341</v>
       </c>
       <c r="D111">
         <v>380</v>
@@ -4780,13 +4780,13 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
+        <v>340</v>
+      </c>
+      <c r="B112" t="s">
+        <v>341</v>
+      </c>
+      <c r="C112" t="s">
         <v>342</v>
-      </c>
-      <c r="B112" t="s">
-        <v>343</v>
-      </c>
-      <c r="C112" t="s">
-        <v>344</v>
       </c>
       <c r="D112">
         <v>388</v>
@@ -4797,13 +4797,13 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
+        <v>343</v>
+      </c>
+      <c r="B113" t="s">
+        <v>344</v>
+      </c>
+      <c r="C113" t="s">
         <v>345</v>
-      </c>
-      <c r="B113" t="s">
-        <v>346</v>
-      </c>
-      <c r="C113" t="s">
-        <v>347</v>
       </c>
       <c r="D113">
         <v>392</v>
@@ -4814,13 +4814,13 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
+        <v>346</v>
+      </c>
+      <c r="B114" t="s">
+        <v>347</v>
+      </c>
+      <c r="C114" t="s">
         <v>348</v>
-      </c>
-      <c r="B114" t="s">
-        <v>349</v>
-      </c>
-      <c r="C114" t="s">
-        <v>350</v>
       </c>
       <c r="D114">
         <v>832</v>
@@ -4831,13 +4831,13 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
+        <v>349</v>
+      </c>
+      <c r="B115" t="s">
+        <v>350</v>
+      </c>
+      <c r="C115" t="s">
         <v>351</v>
-      </c>
-      <c r="B115" t="s">
-        <v>352</v>
-      </c>
-      <c r="C115" t="s">
-        <v>353</v>
       </c>
       <c r="D115">
         <v>400</v>
@@ -4848,13 +4848,13 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
+        <v>352</v>
+      </c>
+      <c r="B116" t="s">
+        <v>353</v>
+      </c>
+      <c r="C116" t="s">
         <v>354</v>
-      </c>
-      <c r="B116" t="s">
-        <v>355</v>
-      </c>
-      <c r="C116" t="s">
-        <v>356</v>
       </c>
       <c r="D116">
         <v>398</v>
@@ -4865,13 +4865,13 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
+        <v>355</v>
+      </c>
+      <c r="B117" t="s">
+        <v>356</v>
+      </c>
+      <c r="C117" t="s">
         <v>357</v>
-      </c>
-      <c r="B117" t="s">
-        <v>358</v>
-      </c>
-      <c r="C117" t="s">
-        <v>359</v>
       </c>
       <c r="D117">
         <v>404</v>
@@ -4882,13 +4882,13 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
+        <v>358</v>
+      </c>
+      <c r="B118" t="s">
+        <v>359</v>
+      </c>
+      <c r="C118" t="s">
         <v>360</v>
-      </c>
-      <c r="B118" t="s">
-        <v>361</v>
-      </c>
-      <c r="C118" t="s">
-        <v>362</v>
       </c>
       <c r="D118">
         <v>296</v>
@@ -4899,19 +4899,19 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
+        <v>361</v>
+      </c>
+      <c r="B119" t="s">
+        <v>362</v>
+      </c>
+      <c r="C119" t="s">
         <v>363</v>
-      </c>
-      <c r="B119" t="s">
-        <v>364</v>
-      </c>
-      <c r="C119" t="s">
-        <v>365</v>
       </c>
       <c r="D119">
         <v>408</v>
       </c>
       <c r="E119" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F119" s="2">
         <v>24213510</v>
@@ -4919,19 +4919,19 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
+        <v>365</v>
+      </c>
+      <c r="B120" t="s">
+        <v>366</v>
+      </c>
+      <c r="C120" t="s">
         <v>367</v>
-      </c>
-      <c r="B120" t="s">
-        <v>368</v>
-      </c>
-      <c r="C120" t="s">
-        <v>369</v>
       </c>
       <c r="D120">
         <v>410</v>
       </c>
       <c r="E120" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F120" s="2">
         <v>50617045</v>
@@ -4939,13 +4939,13 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
+        <v>369</v>
+      </c>
+      <c r="B121" t="s">
+        <v>370</v>
+      </c>
+      <c r="C121" t="s">
         <v>371</v>
-      </c>
-      <c r="B121" t="s">
-        <v>372</v>
-      </c>
-      <c r="C121" t="s">
-        <v>373</v>
       </c>
       <c r="D121">
         <v>414</v>
@@ -4956,13 +4956,13 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
+        <v>372</v>
+      </c>
+      <c r="B122" t="s">
+        <v>373</v>
+      </c>
+      <c r="C122" t="s">
         <v>374</v>
-      </c>
-      <c r="B122" t="s">
-        <v>375</v>
-      </c>
-      <c r="C122" t="s">
-        <v>376</v>
       </c>
       <c r="D122">
         <v>417</v>
@@ -4973,19 +4973,19 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
+        <v>375</v>
+      </c>
+      <c r="B123" t="s">
+        <v>376</v>
+      </c>
+      <c r="C123" t="s">
         <v>377</v>
-      </c>
-      <c r="B123" t="s">
-        <v>378</v>
-      </c>
-      <c r="C123" t="s">
-        <v>379</v>
       </c>
       <c r="D123">
         <v>418</v>
       </c>
       <c r="E123" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F123" s="2">
         <v>6492400</v>
@@ -4993,13 +4993,13 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
+        <v>379</v>
+      </c>
+      <c r="B124" t="s">
+        <v>380</v>
+      </c>
+      <c r="C124" t="s">
         <v>381</v>
-      </c>
-      <c r="B124" t="s">
-        <v>382</v>
-      </c>
-      <c r="C124" t="s">
-        <v>383</v>
       </c>
       <c r="D124">
         <v>428</v>
@@ -5010,13 +5010,13 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
+        <v>382</v>
+      </c>
+      <c r="B125" t="s">
+        <v>383</v>
+      </c>
+      <c r="C125" t="s">
         <v>384</v>
-      </c>
-      <c r="B125" t="s">
-        <v>385</v>
-      </c>
-      <c r="C125" t="s">
-        <v>386</v>
       </c>
       <c r="D125">
         <v>422</v>
@@ -5027,13 +5027,13 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
+        <v>385</v>
+      </c>
+      <c r="B126" t="s">
+        <v>386</v>
+      </c>
+      <c r="C126" t="s">
         <v>387</v>
-      </c>
-      <c r="B126" t="s">
-        <v>388</v>
-      </c>
-      <c r="C126" t="s">
-        <v>389</v>
       </c>
       <c r="D126">
         <v>426</v>
@@ -5044,13 +5044,13 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
+        <v>388</v>
+      </c>
+      <c r="B127" t="s">
+        <v>389</v>
+      </c>
+      <c r="C127" t="s">
         <v>390</v>
-      </c>
-      <c r="B127" t="s">
-        <v>391</v>
-      </c>
-      <c r="C127" t="s">
-        <v>392</v>
       </c>
       <c r="D127">
         <v>430</v>
@@ -5061,13 +5061,13 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
+        <v>391</v>
+      </c>
+      <c r="B128" t="s">
+        <v>392</v>
+      </c>
+      <c r="C128" t="s">
         <v>393</v>
-      </c>
-      <c r="B128" t="s">
-        <v>394</v>
-      </c>
-      <c r="C128" t="s">
-        <v>395</v>
       </c>
       <c r="D128">
         <v>434</v>
@@ -5078,13 +5078,13 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
+        <v>394</v>
+      </c>
+      <c r="B129" t="s">
+        <v>395</v>
+      </c>
+      <c r="C129" t="s">
         <v>396</v>
-      </c>
-      <c r="B129" t="s">
-        <v>397</v>
-      </c>
-      <c r="C129" t="s">
-        <v>398</v>
       </c>
       <c r="D129">
         <v>438</v>
@@ -5095,13 +5095,13 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
+        <v>397</v>
+      </c>
+      <c r="B130" t="s">
+        <v>398</v>
+      </c>
+      <c r="C130" t="s">
         <v>399</v>
-      </c>
-      <c r="B130" t="s">
-        <v>400</v>
-      </c>
-      <c r="C130" t="s">
-        <v>401</v>
       </c>
       <c r="D130">
         <v>440</v>
@@ -5112,13 +5112,13 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
+        <v>400</v>
+      </c>
+      <c r="B131" t="s">
+        <v>401</v>
+      </c>
+      <c r="C131" t="s">
         <v>402</v>
-      </c>
-      <c r="B131" t="s">
-        <v>403</v>
-      </c>
-      <c r="C131" t="s">
-        <v>404</v>
       </c>
       <c r="D131">
         <v>442</v>
@@ -5129,13 +5129,13 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
+        <v>403</v>
+      </c>
+      <c r="B132" t="s">
+        <v>404</v>
+      </c>
+      <c r="C132" t="s">
         <v>405</v>
-      </c>
-      <c r="B132" t="s">
-        <v>406</v>
-      </c>
-      <c r="C132" t="s">
-        <v>407</v>
       </c>
       <c r="D132">
         <v>446</v>
@@ -5146,19 +5146,19 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
+        <v>406</v>
+      </c>
+      <c r="B133" t="s">
+        <v>407</v>
+      </c>
+      <c r="C133" t="s">
         <v>408</v>
-      </c>
-      <c r="B133" t="s">
-        <v>409</v>
-      </c>
-      <c r="C133" t="s">
-        <v>410</v>
       </c>
       <c r="D133">
         <v>807</v>
       </c>
       <c r="E133" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F133" s="2">
         <v>2071278</v>
@@ -5166,13 +5166,13 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
+        <v>410</v>
+      </c>
+      <c r="B134" t="s">
+        <v>411</v>
+      </c>
+      <c r="C134" t="s">
         <v>412</v>
-      </c>
-      <c r="B134" t="s">
-        <v>413</v>
-      </c>
-      <c r="C134" t="s">
-        <v>414</v>
       </c>
       <c r="D134">
         <v>450</v>
@@ -5183,13 +5183,13 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
+        <v>413</v>
+      </c>
+      <c r="B135" t="s">
+        <v>414</v>
+      </c>
+      <c r="C135" t="s">
         <v>415</v>
-      </c>
-      <c r="B135" t="s">
-        <v>416</v>
-      </c>
-      <c r="C135" t="s">
-        <v>417</v>
       </c>
       <c r="D135">
         <v>454</v>
@@ -5200,13 +5200,13 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
+        <v>416</v>
+      </c>
+      <c r="B136" t="s">
+        <v>417</v>
+      </c>
+      <c r="C136" t="s">
         <v>418</v>
-      </c>
-      <c r="B136" t="s">
-        <v>419</v>
-      </c>
-      <c r="C136" t="s">
-        <v>420</v>
       </c>
       <c r="D136">
         <v>458</v>
@@ -5217,13 +5217,13 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
+        <v>419</v>
+      </c>
+      <c r="B137" t="s">
+        <v>420</v>
+      </c>
+      <c r="C137" t="s">
         <v>421</v>
-      </c>
-      <c r="B137" t="s">
-        <v>422</v>
-      </c>
-      <c r="C137" t="s">
-        <v>423</v>
       </c>
       <c r="D137">
         <v>462</v>
@@ -5234,13 +5234,13 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
+        <v>422</v>
+      </c>
+      <c r="B138" t="s">
+        <v>423</v>
+      </c>
+      <c r="C138" t="s">
         <v>424</v>
-      </c>
-      <c r="B138" t="s">
-        <v>425</v>
-      </c>
-      <c r="C138" t="s">
-        <v>426</v>
       </c>
       <c r="D138">
         <v>466</v>
@@ -5251,13 +5251,13 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
+        <v>425</v>
+      </c>
+      <c r="B139" t="s">
+        <v>426</v>
+      </c>
+      <c r="C139" t="s">
         <v>427</v>
-      </c>
-      <c r="B139" t="s">
-        <v>428</v>
-      </c>
-      <c r="C139" t="s">
-        <v>429</v>
       </c>
       <c r="D139">
         <v>470</v>
@@ -5268,13 +5268,13 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
+        <v>428</v>
+      </c>
+      <c r="B140" t="s">
+        <v>429</v>
+      </c>
+      <c r="C140" t="s">
         <v>430</v>
-      </c>
-      <c r="B140" t="s">
-        <v>431</v>
-      </c>
-      <c r="C140" t="s">
-        <v>432</v>
       </c>
       <c r="D140">
         <v>584</v>
@@ -5285,13 +5285,13 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
+        <v>431</v>
+      </c>
+      <c r="B141" t="s">
+        <v>432</v>
+      </c>
+      <c r="C141" t="s">
         <v>433</v>
-      </c>
-      <c r="B141" t="s">
-        <v>434</v>
-      </c>
-      <c r="C141" t="s">
-        <v>435</v>
       </c>
       <c r="D141">
         <v>474</v>
@@ -5302,13 +5302,13 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
+        <v>434</v>
+      </c>
+      <c r="B142" t="s">
+        <v>435</v>
+      </c>
+      <c r="C142" t="s">
         <v>436</v>
-      </c>
-      <c r="B142" t="s">
-        <v>437</v>
-      </c>
-      <c r="C142" t="s">
-        <v>438</v>
       </c>
       <c r="D142">
         <v>478</v>
@@ -5319,13 +5319,13 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
+        <v>437</v>
+      </c>
+      <c r="B143" t="s">
+        <v>438</v>
+      </c>
+      <c r="C143" t="s">
         <v>439</v>
-      </c>
-      <c r="B143" t="s">
-        <v>440</v>
-      </c>
-      <c r="C143" t="s">
-        <v>441</v>
       </c>
       <c r="D143">
         <v>480</v>
@@ -5336,13 +5336,13 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
+        <v>440</v>
+      </c>
+      <c r="B144" t="s">
+        <v>441</v>
+      </c>
+      <c r="C144" t="s">
         <v>442</v>
-      </c>
-      <c r="B144" t="s">
-        <v>443</v>
-      </c>
-      <c r="C144" t="s">
-        <v>444</v>
       </c>
       <c r="D144">
         <v>175</v>
@@ -5353,13 +5353,13 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
+        <v>443</v>
+      </c>
+      <c r="B145" t="s">
+        <v>444</v>
+      </c>
+      <c r="C145" t="s">
         <v>445</v>
-      </c>
-      <c r="B145" t="s">
-        <v>446</v>
-      </c>
-      <c r="C145" t="s">
-        <v>447</v>
       </c>
       <c r="D145">
         <v>484</v>
@@ -5370,13 +5370,13 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
+        <v>446</v>
+      </c>
+      <c r="B146" t="s">
+        <v>447</v>
+      </c>
+      <c r="C146" t="s">
         <v>448</v>
-      </c>
-      <c r="B146" t="s">
-        <v>449</v>
-      </c>
-      <c r="C146" t="s">
-        <v>450</v>
       </c>
       <c r="D146">
         <v>583</v>
@@ -5387,19 +5387,19 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
+        <v>449</v>
+      </c>
+      <c r="B147" t="s">
+        <v>450</v>
+      </c>
+      <c r="C147" t="s">
         <v>451</v>
-      </c>
-      <c r="B147" t="s">
-        <v>452</v>
-      </c>
-      <c r="C147" t="s">
-        <v>453</v>
       </c>
       <c r="D147">
         <v>498</v>
       </c>
       <c r="E147" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F147" s="2">
         <v>3553100</v>
@@ -5407,13 +5407,13 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
+        <v>453</v>
+      </c>
+      <c r="B148" t="s">
+        <v>454</v>
+      </c>
+      <c r="C148" t="s">
         <v>455</v>
-      </c>
-      <c r="B148" t="s">
-        <v>456</v>
-      </c>
-      <c r="C148" t="s">
-        <v>457</v>
       </c>
       <c r="D148">
         <v>492</v>
@@ -5424,13 +5424,13 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
+        <v>456</v>
+      </c>
+      <c r="B149" t="s">
+        <v>457</v>
+      </c>
+      <c r="C149" t="s">
         <v>458</v>
-      </c>
-      <c r="B149" t="s">
-        <v>459</v>
-      </c>
-      <c r="C149" t="s">
-        <v>460</v>
       </c>
       <c r="D149">
         <v>496</v>
@@ -5441,13 +5441,13 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
+        <v>459</v>
+      </c>
+      <c r="B150" t="s">
+        <v>460</v>
+      </c>
+      <c r="C150" t="s">
         <v>461</v>
-      </c>
-      <c r="B150" t="s">
-        <v>462</v>
-      </c>
-      <c r="C150" t="s">
-        <v>463</v>
       </c>
       <c r="D150">
         <v>499</v>
@@ -5458,13 +5458,13 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
+        <v>462</v>
+      </c>
+      <c r="B151" t="s">
+        <v>463</v>
+      </c>
+      <c r="C151" t="s">
         <v>464</v>
-      </c>
-      <c r="B151" t="s">
-        <v>465</v>
-      </c>
-      <c r="C151" t="s">
-        <v>466</v>
       </c>
       <c r="D151">
         <v>500</v>
@@ -5475,13 +5475,13 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
+        <v>465</v>
+      </c>
+      <c r="B152" t="s">
+        <v>466</v>
+      </c>
+      <c r="C152" t="s">
         <v>467</v>
-      </c>
-      <c r="B152" t="s">
-        <v>468</v>
-      </c>
-      <c r="C152" t="s">
-        <v>469</v>
       </c>
       <c r="D152">
         <v>504</v>
@@ -5492,13 +5492,13 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
+        <v>468</v>
+      </c>
+      <c r="B153" t="s">
+        <v>469</v>
+      </c>
+      <c r="C153" t="s">
         <v>470</v>
-      </c>
-      <c r="B153" t="s">
-        <v>471</v>
-      </c>
-      <c r="C153" t="s">
-        <v>472</v>
       </c>
       <c r="D153">
         <v>508</v>
@@ -5509,13 +5509,13 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
+        <v>471</v>
+      </c>
+      <c r="B154" t="s">
+        <v>472</v>
+      </c>
+      <c r="C154" t="s">
         <v>473</v>
-      </c>
-      <c r="B154" t="s">
-        <v>474</v>
-      </c>
-      <c r="C154" t="s">
-        <v>475</v>
       </c>
       <c r="D154">
         <v>104</v>
@@ -5526,13 +5526,13 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
+        <v>474</v>
+      </c>
+      <c r="B155" t="s">
+        <v>475</v>
+      </c>
+      <c r="C155" t="s">
         <v>476</v>
-      </c>
-      <c r="B155" t="s">
-        <v>477</v>
-      </c>
-      <c r="C155" t="s">
-        <v>478</v>
       </c>
       <c r="D155">
         <v>516</v>
@@ -5543,13 +5543,13 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
+        <v>477</v>
+      </c>
+      <c r="B156" t="s">
+        <v>478</v>
+      </c>
+      <c r="C156" t="s">
         <v>479</v>
-      </c>
-      <c r="B156" t="s">
-        <v>480</v>
-      </c>
-      <c r="C156" t="s">
-        <v>481</v>
       </c>
       <c r="D156">
         <v>520</v>
@@ -5560,13 +5560,13 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
+        <v>480</v>
+      </c>
+      <c r="B157" t="s">
+        <v>481</v>
+      </c>
+      <c r="C157" t="s">
         <v>482</v>
-      </c>
-      <c r="B157" t="s">
-        <v>483</v>
-      </c>
-      <c r="C157" t="s">
-        <v>484</v>
       </c>
       <c r="D157">
         <v>524</v>
@@ -5577,13 +5577,13 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
+        <v>483</v>
+      </c>
+      <c r="B158" t="s">
+        <v>484</v>
+      </c>
+      <c r="C158" t="s">
         <v>485</v>
-      </c>
-      <c r="B158" t="s">
-        <v>486</v>
-      </c>
-      <c r="C158" t="s">
-        <v>487</v>
       </c>
       <c r="D158">
         <v>528</v>
@@ -5594,13 +5594,13 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
+        <v>486</v>
+      </c>
+      <c r="B159" t="s">
+        <v>487</v>
+      </c>
+      <c r="C159" t="s">
         <v>488</v>
-      </c>
-      <c r="B159" t="s">
-        <v>489</v>
-      </c>
-      <c r="C159" t="s">
-        <v>490</v>
       </c>
       <c r="D159">
         <v>540</v>
@@ -5611,13 +5611,13 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
+        <v>489</v>
+      </c>
+      <c r="B160" t="s">
+        <v>490</v>
+      </c>
+      <c r="C160" t="s">
         <v>491</v>
-      </c>
-      <c r="B160" t="s">
-        <v>492</v>
-      </c>
-      <c r="C160" t="s">
-        <v>493</v>
       </c>
       <c r="D160">
         <v>554</v>
@@ -5628,13 +5628,13 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
+        <v>492</v>
+      </c>
+      <c r="B161" t="s">
+        <v>493</v>
+      </c>
+      <c r="C161" t="s">
         <v>494</v>
-      </c>
-      <c r="B161" t="s">
-        <v>495</v>
-      </c>
-      <c r="C161" t="s">
-        <v>496</v>
       </c>
       <c r="D161">
         <v>558</v>
@@ -5645,13 +5645,13 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
+        <v>495</v>
+      </c>
+      <c r="B162" t="s">
+        <v>496</v>
+      </c>
+      <c r="C162" t="s">
         <v>497</v>
-      </c>
-      <c r="B162" t="s">
-        <v>498</v>
-      </c>
-      <c r="C162" t="s">
-        <v>499</v>
       </c>
       <c r="D162">
         <v>562</v>
@@ -5662,13 +5662,13 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
+        <v>498</v>
+      </c>
+      <c r="B163" t="s">
+        <v>499</v>
+      </c>
+      <c r="C163" t="s">
         <v>500</v>
-      </c>
-      <c r="B163" t="s">
-        <v>501</v>
-      </c>
-      <c r="C163" t="s">
-        <v>502</v>
       </c>
       <c r="D163">
         <v>566</v>
@@ -5679,13 +5679,13 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
+        <v>501</v>
+      </c>
+      <c r="B164" t="s">
+        <v>502</v>
+      </c>
+      <c r="C164" t="s">
         <v>503</v>
-      </c>
-      <c r="B164" t="s">
-        <v>504</v>
-      </c>
-      <c r="C164" t="s">
-        <v>505</v>
       </c>
       <c r="D164">
         <v>570</v>
@@ -5696,13 +5696,13 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
+        <v>504</v>
+      </c>
+      <c r="B165" t="s">
+        <v>505</v>
+      </c>
+      <c r="C165" t="s">
         <v>506</v>
-      </c>
-      <c r="B165" t="s">
-        <v>507</v>
-      </c>
-      <c r="C165" t="s">
-        <v>508</v>
       </c>
       <c r="D165">
         <v>574</v>
@@ -5713,13 +5713,13 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
+        <v>507</v>
+      </c>
+      <c r="B166" t="s">
+        <v>508</v>
+      </c>
+      <c r="C166" t="s">
         <v>509</v>
-      </c>
-      <c r="B166" t="s">
-        <v>510</v>
-      </c>
-      <c r="C166" t="s">
-        <v>511</v>
       </c>
       <c r="D166">
         <v>580</v>
@@ -5730,13 +5730,13 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
+        <v>510</v>
+      </c>
+      <c r="B167" t="s">
+        <v>511</v>
+      </c>
+      <c r="C167" t="s">
         <v>512</v>
-      </c>
-      <c r="B167" t="s">
-        <v>513</v>
-      </c>
-      <c r="C167" t="s">
-        <v>514</v>
       </c>
       <c r="D167">
         <v>578</v>
@@ -5747,13 +5747,13 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
+        <v>513</v>
+      </c>
+      <c r="B168" t="s">
+        <v>514</v>
+      </c>
+      <c r="C168" t="s">
         <v>515</v>
-      </c>
-      <c r="B168" t="s">
-        <v>516</v>
-      </c>
-      <c r="C168" t="s">
-        <v>517</v>
       </c>
       <c r="D168">
         <v>512</v>
@@ -5764,13 +5764,13 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
+        <v>516</v>
+      </c>
+      <c r="B169" t="s">
+        <v>517</v>
+      </c>
+      <c r="C169" t="s">
         <v>518</v>
-      </c>
-      <c r="B169" t="s">
-        <v>519</v>
-      </c>
-      <c r="C169" t="s">
-        <v>520</v>
       </c>
       <c r="D169">
         <v>586</v>
@@ -5781,13 +5781,13 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
+        <v>519</v>
+      </c>
+      <c r="B170" t="s">
+        <v>520</v>
+      </c>
+      <c r="C170" t="s">
         <v>521</v>
-      </c>
-      <c r="B170" t="s">
-        <v>522</v>
-      </c>
-      <c r="C170" t="s">
-        <v>523</v>
       </c>
       <c r="D170">
         <v>585</v>
@@ -5798,19 +5798,19 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
+        <v>522</v>
+      </c>
+      <c r="B171" t="s">
+        <v>523</v>
+      </c>
+      <c r="C171" t="s">
         <v>524</v>
-      </c>
-      <c r="B171" t="s">
-        <v>525</v>
-      </c>
-      <c r="C171" t="s">
-        <v>526</v>
       </c>
       <c r="D171">
         <v>275</v>
       </c>
       <c r="E171" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F171" s="2">
         <v>4816503</v>
@@ -5818,13 +5818,13 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
+        <v>526</v>
+      </c>
+      <c r="B172" t="s">
+        <v>527</v>
+      </c>
+      <c r="C172" t="s">
         <v>528</v>
-      </c>
-      <c r="B172" t="s">
-        <v>529</v>
-      </c>
-      <c r="C172" t="s">
-        <v>530</v>
       </c>
       <c r="D172">
         <v>591</v>
@@ -5835,13 +5835,13 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
+        <v>529</v>
+      </c>
+      <c r="B173" t="s">
+        <v>530</v>
+      </c>
+      <c r="C173" t="s">
         <v>531</v>
-      </c>
-      <c r="B173" t="s">
-        <v>532</v>
-      </c>
-      <c r="C173" t="s">
-        <v>533</v>
       </c>
       <c r="D173">
         <v>598</v>
@@ -5852,13 +5852,13 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
+        <v>532</v>
+      </c>
+      <c r="B174" t="s">
+        <v>533</v>
+      </c>
+      <c r="C174" t="s">
         <v>534</v>
-      </c>
-      <c r="B174" t="s">
-        <v>535</v>
-      </c>
-      <c r="C174" t="s">
-        <v>536</v>
       </c>
       <c r="D174">
         <v>600</v>
@@ -5869,13 +5869,13 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
+        <v>535</v>
+      </c>
+      <c r="B175" t="s">
+        <v>536</v>
+      </c>
+      <c r="C175" t="s">
         <v>537</v>
-      </c>
-      <c r="B175" t="s">
-        <v>538</v>
-      </c>
-      <c r="C175" t="s">
-        <v>539</v>
       </c>
       <c r="D175">
         <v>604</v>
@@ -5886,13 +5886,13 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
+        <v>538</v>
+      </c>
+      <c r="B176" t="s">
+        <v>539</v>
+      </c>
+      <c r="C176" t="s">
         <v>540</v>
-      </c>
-      <c r="B176" t="s">
-        <v>541</v>
-      </c>
-      <c r="C176" t="s">
-        <v>542</v>
       </c>
       <c r="D176">
         <v>608</v>
@@ -5903,13 +5903,13 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
+        <v>541</v>
+      </c>
+      <c r="B177" t="s">
+        <v>542</v>
+      </c>
+      <c r="C177" t="s">
         <v>543</v>
-      </c>
-      <c r="B177" t="s">
-        <v>544</v>
-      </c>
-      <c r="C177" t="s">
-        <v>545</v>
       </c>
       <c r="D177">
         <v>612</v>
@@ -5920,13 +5920,13 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
+        <v>544</v>
+      </c>
+      <c r="B178" t="s">
+        <v>545</v>
+      </c>
+      <c r="C178" t="s">
         <v>546</v>
-      </c>
-      <c r="B178" t="s">
-        <v>547</v>
-      </c>
-      <c r="C178" t="s">
-        <v>548</v>
       </c>
       <c r="D178">
         <v>616</v>
@@ -5937,13 +5937,13 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
+        <v>547</v>
+      </c>
+      <c r="B179" t="s">
+        <v>548</v>
+      </c>
+      <c r="C179" t="s">
         <v>549</v>
-      </c>
-      <c r="B179" t="s">
-        <v>550</v>
-      </c>
-      <c r="C179" t="s">
-        <v>551</v>
       </c>
       <c r="D179">
         <v>620</v>
@@ -5954,13 +5954,13 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
+        <v>550</v>
+      </c>
+      <c r="B180" t="s">
+        <v>551</v>
+      </c>
+      <c r="C180" t="s">
         <v>552</v>
-      </c>
-      <c r="B180" t="s">
-        <v>553</v>
-      </c>
-      <c r="C180" t="s">
-        <v>554</v>
       </c>
       <c r="D180">
         <v>630</v>
@@ -5971,13 +5971,13 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
+        <v>553</v>
+      </c>
+      <c r="B181" t="s">
+        <v>554</v>
+      </c>
+      <c r="C181" t="s">
         <v>555</v>
-      </c>
-      <c r="B181" t="s">
-        <v>556</v>
-      </c>
-      <c r="C181" t="s">
-        <v>557</v>
       </c>
       <c r="D181">
         <v>634</v>
@@ -5988,13 +5988,13 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
+        <v>556</v>
+      </c>
+      <c r="B182" t="s">
+        <v>557</v>
+      </c>
+      <c r="C182" t="s">
         <v>558</v>
-      </c>
-      <c r="B182" t="s">
-        <v>559</v>
-      </c>
-      <c r="C182" t="s">
-        <v>560</v>
       </c>
       <c r="D182">
         <v>638</v>
@@ -6005,13 +6005,13 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" t="s">
+        <v>559</v>
+      </c>
+      <c r="B183" t="s">
+        <v>560</v>
+      </c>
+      <c r="C183" t="s">
         <v>561</v>
-      </c>
-      <c r="B183" t="s">
-        <v>562</v>
-      </c>
-      <c r="C183" t="s">
-        <v>563</v>
       </c>
       <c r="D183">
         <v>642</v>
@@ -6022,19 +6022,19 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
+        <v>562</v>
+      </c>
+      <c r="B184" t="s">
+        <v>563</v>
+      </c>
+      <c r="C184" t="s">
         <v>564</v>
-      </c>
-      <c r="B184" t="s">
-        <v>565</v>
-      </c>
-      <c r="C184" t="s">
-        <v>566</v>
       </c>
       <c r="D184">
         <v>643</v>
       </c>
       <c r="E184" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F184" s="2">
         <v>146654366</v>
@@ -6042,13 +6042,13 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
+        <v>566</v>
+      </c>
+      <c r="B185" t="s">
+        <v>567</v>
+      </c>
+      <c r="C185" t="s">
         <v>568</v>
-      </c>
-      <c r="B185" t="s">
-        <v>569</v>
-      </c>
-      <c r="C185" t="s">
-        <v>570</v>
       </c>
       <c r="D185">
         <v>646</v>
@@ -6059,13 +6059,13 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
-        <v>571</v>
+        <v>784</v>
       </c>
       <c r="B186" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C186" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D186">
         <v>652</v>
@@ -6076,19 +6076,19 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B187" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C187" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D187">
         <v>654</v>
       </c>
       <c r="E187" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F187" s="2">
         <v>4255</v>
@@ -6096,13 +6096,13 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B188" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C188" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D188">
         <v>659</v>
@@ -6113,13 +6113,13 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B189" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C189" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D189">
         <v>662</v>
@@ -6130,13 +6130,13 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B190" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C190" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D190">
         <v>663</v>
@@ -6147,13 +6147,13 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B191" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C191" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D191">
         <v>666</v>
@@ -6164,13 +6164,13 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B192" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C192" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D192">
         <v>670</v>
@@ -6181,13 +6181,13 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B193" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C193" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D193">
         <v>882</v>
@@ -6198,13 +6198,13 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B194" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C194" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D194">
         <v>674</v>
@@ -6215,13 +6215,13 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B195" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C195" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D195">
         <v>678</v>
@@ -6232,13 +6232,13 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B196" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C196" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D196">
         <v>682</v>
@@ -6249,13 +6249,13 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B197" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C197" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D197">
         <v>686</v>
@@ -6266,13 +6266,13 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B198" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C198" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D198">
         <v>688</v>
@@ -6283,13 +6283,13 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B199" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C199" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D199">
         <v>690</v>
@@ -6300,13 +6300,13 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B200" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C200" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D200">
         <v>694</v>
@@ -6317,13 +6317,13 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B201" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C201" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D201">
         <v>702</v>
@@ -6334,13 +6334,13 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B202" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C202" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D202">
         <v>534</v>
@@ -6351,13 +6351,13 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B203" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C203" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D203">
         <v>703</v>
@@ -6368,13 +6368,13 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B204" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C204" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D204">
         <v>705</v>
@@ -6385,13 +6385,13 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B205" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C205" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D205">
         <v>90</v>
@@ -6402,13 +6402,13 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B206" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C206" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D206">
         <v>706</v>
@@ -6419,13 +6419,13 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B207" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C207" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D207">
         <v>710</v>
@@ -6436,13 +6436,13 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B208" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C208" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D208">
         <v>239</v>
@@ -6453,13 +6453,13 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B209" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C209" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D209">
         <v>728</v>
@@ -6470,13 +6470,13 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B210" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C210" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D210">
         <v>724</v>
@@ -6487,13 +6487,13 @@
     </row>
     <row r="211" spans="1:6">
       <c r="A211" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B211" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C211" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D211">
         <v>144</v>
@@ -6504,13 +6504,13 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B212" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C212" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="D212">
         <v>729</v>
@@ -6521,13 +6521,13 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B213" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C213" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D213">
         <v>740</v>
@@ -6538,13 +6538,13 @@
     </row>
     <row r="214" spans="1:6">
       <c r="A214" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B214" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C214" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D214">
         <v>744</v>
@@ -6555,13 +6555,13 @@
     </row>
     <row r="215" spans="1:6">
       <c r="A215" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B215" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C215" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D215">
         <v>748</v>
@@ -6572,13 +6572,13 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B216" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C216" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D216">
         <v>752</v>
@@ -6589,13 +6589,13 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B217" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C217" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D217">
         <v>756</v>
@@ -6606,19 +6606,19 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="B218" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C218" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D218">
         <v>760</v>
       </c>
       <c r="E218" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="F218" s="2">
         <v>18564000</v>
@@ -6626,13 +6626,13 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B219" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C219" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D219">
         <v>158</v>
@@ -6643,13 +6643,13 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B220" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C220" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D220">
         <v>762</v>
@@ -6660,19 +6660,19 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B221" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C221" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D221">
         <v>834</v>
       </c>
       <c r="E221" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="F221" s="2">
         <v>55155000</v>
@@ -6680,13 +6680,13 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="B222" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="C222" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D222">
         <v>764</v>
@@ -6697,13 +6697,13 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="B223" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C223" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D223">
         <v>626</v>
@@ -6714,13 +6714,13 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B224" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C224" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D224">
         <v>768</v>
@@ -6731,13 +6731,13 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B225" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C225" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D225">
         <v>772</v>
@@ -6748,13 +6748,13 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B226" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C226" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D226">
         <v>776</v>
@@ -6765,13 +6765,13 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B227" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="C227" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D227">
         <v>780</v>
@@ -6782,13 +6782,13 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B228" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C228" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D228">
         <v>788</v>
@@ -6799,13 +6799,13 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B229" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C229" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D229">
         <v>792</v>
@@ -6816,13 +6816,13 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B230" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C230" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D230">
         <v>795</v>
@@ -6833,13 +6833,13 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B231" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C231" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D231">
         <v>796</v>
@@ -6850,13 +6850,13 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B232" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="C232" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="D232">
         <v>798</v>
@@ -6867,13 +6867,13 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B233" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C233" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D233">
         <v>800</v>
@@ -6884,13 +6884,13 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B234" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C234" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D234">
         <v>804</v>
@@ -6901,13 +6901,13 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B235" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="C235" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D235">
         <v>784</v>
@@ -6918,13 +6918,13 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B236" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C236" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="D236">
         <v>826</v>
@@ -6935,13 +6935,13 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B237" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C237" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="D237">
         <v>840</v>
@@ -6952,13 +6952,13 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="B238" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C238" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D238">
         <v>581</v>
@@ -6969,13 +6969,13 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="B239" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C239" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D239">
         <v>858</v>
@@ -6986,13 +6986,13 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B240" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="C240" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D240">
         <v>860</v>
@@ -7003,13 +7003,13 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="B241" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C241" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D241">
         <v>548</v>
@@ -7020,19 +7020,19 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="B242" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C242" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D242">
         <v>862</v>
       </c>
       <c r="E242" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="F242" s="2">
         <v>31028700</v>
@@ -7040,13 +7040,13 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="B243" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C243" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="D243">
         <v>704</v>
@@ -7057,13 +7057,13 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B244" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="C244" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="D244">
         <v>92</v>
@@ -7074,13 +7074,13 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B245" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="C245" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D245">
         <v>850</v>
@@ -7091,13 +7091,13 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B246" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C246" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D246">
         <v>876</v>
@@ -7108,13 +7108,13 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="B247" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="C247" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D247">
         <v>732</v>
@@ -7125,13 +7125,13 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="B248" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="C248" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D248">
         <v>887</v>
@@ -7142,13 +7142,13 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B249" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="C249" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D249">
         <v>894</v>
@@ -7159,13 +7159,13 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B250" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C250" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D250">
         <v>716</v>
@@ -7176,70 +7176,70 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="B251" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="C251" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D251">
         <v>902</v>
       </c>
       <c r="E251" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="252" spans="1:6">
       <c r="A252" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="B252" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="C252" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D252">
         <v>903</v>
       </c>
       <c r="E252" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="253" spans="1:6">
       <c r="A253" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="B253" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C253" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D253">
         <v>904</v>
       </c>
       <c r="E253" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="254" spans="1:6">
       <c r="A254" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="B254" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C254" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D254">
         <v>0</v>
       </c>
       <c r="E254" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="F254" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed population exposure formatting, and modified country spreadsheet to have namibia 'NA' have quotes around it to prevent pandas from interpreting it as a NaN.
</commit_message>
<xml_diff>
--- a/losspager/data/countries.xlsx
+++ b/losspager/data/countries.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhearne/src/python/losspager/losspager/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="4220" yWindow="1300" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1466,9 +1474,6 @@
     <t>Namibia</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>NAM</t>
   </si>
   <si>
@@ -2394,6 +2399,9 @@
   </si>
   <si>
     <t>Saint Barthelemy</t>
+  </si>
+  <si>
+    <t>"NA"</t>
   </si>
 </sst>
 </file>
@@ -2525,6 +2533,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2856,11 +2869,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
@@ -2870,7 +2883,7 @@
     <col min="6" max="6" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2890,7 +2903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2907,7 +2920,7 @@
         <v>27657145</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2924,7 +2937,7 @@
         <v>29013</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2941,7 +2954,7 @@
         <v>2886026</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2958,7 +2971,7 @@
         <v>40400000</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2975,7 +2988,7 @@
         <v>57100</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2992,7 +3005,7 @@
         <v>78014</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3009,7 +3022,7 @@
         <v>25789024</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3026,7 +3039,7 @@
         <v>13452</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3043,7 +3056,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3060,7 +3073,7 @@
         <v>86295</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3077,7 +3090,7 @@
         <v>43590400</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -3094,7 +3107,7 @@
         <v>2995100</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -3111,7 +3124,7 @@
         <v>110108</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -3128,7 +3141,7 @@
         <v>24192700</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -3145,7 +3158,7 @@
         <v>8741753</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -3162,7 +3175,7 @@
         <v>9755500</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3179,7 +3192,7 @@
         <v>378040</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -3196,7 +3209,7 @@
         <v>1404900</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -3213,7 +3226,7 @@
         <v>161109000</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -3230,7 +3243,7 @@
         <v>285000</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3247,7 +3260,7 @@
         <v>9500000</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -3264,7 +3277,7 @@
         <v>11323925</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -3281,7 +3294,7 @@
         <v>375909</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -3298,7 +3311,7 @@
         <v>10653654</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -3315,7 +3328,7 @@
         <v>61954</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -3332,7 +3345,7 @@
         <v>778210</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -3352,7 +3365,7 @@
         <v>10985059</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -3372,7 +3385,7 @@
         <v>18905</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -3389,7 +3402,7 @@
         <v>3531159</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -3406,7 +3419,7 @@
         <v>2230905</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -3423,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -3440,7 +3453,7 @@
         <v>206678000</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -3457,7 +3470,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>107</v>
       </c>
@@ -3477,7 +3490,7 @@
         <v>411900</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -3494,7 +3507,7 @@
         <v>7153784</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -3511,7 +3524,7 @@
         <v>19034397</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -3528,7 +3541,7 @@
         <v>10114505</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -3545,7 +3558,7 @@
         <v>15626444</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -3562,7 +3575,7 @@
         <v>22709892</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>126</v>
       </c>
@@ -3579,7 +3592,7 @@
         <v>36532600</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>129</v>
       </c>
@@ -3596,7 +3609,7 @@
         <v>531239</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>132</v>
       </c>
@@ -3613,7 +3626,7 @@
         <v>60413</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>135</v>
       </c>
@@ -3630,7 +3643,7 @@
         <v>4998000</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -3647,7 +3660,7 @@
         <v>14497000</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>141</v>
       </c>
@@ -3664,7 +3677,7 @@
         <v>18191900</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -3681,7 +3694,7 @@
         <v>1378840000</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -3698,7 +3711,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>150</v>
       </c>
@@ -3715,7 +3728,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>153</v>
       </c>
@@ -3732,7 +3745,7 @@
         <v>48843300</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -3749,7 +3762,7 @@
         <v>806153</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>159</v>
       </c>
@@ -3766,7 +3779,7 @@
         <v>4741000</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>162</v>
       </c>
@@ -3786,7 +3799,7 @@
         <v>82310000</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -3803,7 +3816,7 @@
         <v>18100</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -3820,9 +3833,9 @@
         <v>4890379</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B56" t="s">
         <v>172</v>
@@ -3837,7 +3850,7 @@
         <v>22671331</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -3854,7 +3867,7 @@
         <v>4190669</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>177</v>
       </c>
@@ -3871,9 +3884,9 @@
         <v>11239004</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B59" t="s">
         <v>180</v>
@@ -3888,7 +3901,7 @@
         <v>158986</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -3905,7 +3918,7 @@
         <v>847000</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -3922,7 +3935,7 @@
         <v>10558524</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>188</v>
       </c>
@@ -3939,7 +3952,7 @@
         <v>5724456</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>191</v>
       </c>
@@ -3956,7 +3969,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>194</v>
       </c>
@@ -3973,7 +3986,7 @@
         <v>71293</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -3990,7 +4003,7 @@
         <v>10075045</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -4007,7 +4020,7 @@
         <v>16618231</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -4024,7 +4037,7 @@
         <v>91610300</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>206</v>
       </c>
@@ -4041,7 +4054,7 @@
         <v>6520675</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>209</v>
       </c>
@@ -4058,7 +4071,7 @@
         <v>1222442</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>212</v>
       </c>
@@ -4075,7 +4088,7 @@
         <v>5352000</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -4092,7 +4105,7 @@
         <v>1315944</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>218</v>
       </c>
@@ -4109,7 +4122,7 @@
         <v>92206005</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>221</v>
       </c>
@@ -4126,7 +4139,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>224</v>
       </c>
@@ -4143,7 +4156,7 @@
         <v>49552</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>227</v>
       </c>
@@ -4160,7 +4173,7 @@
         <v>867000</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>230</v>
       </c>
@@ -4177,7 +4190,7 @@
         <v>5495830</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>233</v>
       </c>
@@ -4194,7 +4207,7 @@
         <v>66763000</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>236</v>
       </c>
@@ -4211,7 +4224,7 @@
         <v>254541</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>239</v>
       </c>
@@ -4228,7 +4241,7 @@
         <v>271800</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>242</v>
       </c>
@@ -4245,7 +4258,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>245</v>
       </c>
@@ -4262,7 +4275,7 @@
         <v>1802278</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>248</v>
       </c>
@@ -4279,7 +4292,7 @@
         <v>1882450</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>251</v>
       </c>
@@ -4296,7 +4309,7 @@
         <v>3720400</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>254</v>
       </c>
@@ -4313,7 +4326,7 @@
         <v>82175700</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>257</v>
       </c>
@@ -4330,7 +4343,7 @@
         <v>27670174</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>260</v>
       </c>
@@ -4347,7 +4360,7 @@
         <v>33140</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>263</v>
       </c>
@@ -4364,7 +4377,7 @@
         <v>10858018</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>266</v>
       </c>
@@ -4381,7 +4394,7 @@
         <v>56186</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>269</v>
       </c>
@@ -4398,7 +4411,7 @@
         <v>103328</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>272</v>
       </c>
@@ -4415,7 +4428,7 @@
         <v>400132</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>275</v>
       </c>
@@ -4432,7 +4445,7 @@
         <v>184200</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>278</v>
       </c>
@@ -4449,7 +4462,7 @@
         <v>16176133</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>281</v>
       </c>
@@ -4466,7 +4479,7 @@
         <v>63001</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>284</v>
       </c>
@@ -4483,7 +4496,7 @@
         <v>12947000</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>287</v>
       </c>
@@ -4500,7 +4513,7 @@
         <v>1547777</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>290</v>
       </c>
@@ -4517,7 +4530,7 @@
         <v>746900</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>293</v>
       </c>
@@ -4534,7 +4547,7 @@
         <v>11078033</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>296</v>
       </c>
@@ -4551,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -4571,7 +4584,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>303</v>
       </c>
@@ -4588,7 +4601,7 @@
         <v>8721014</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>306</v>
       </c>
@@ -4605,7 +4618,7 @@
         <v>7346700</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>309</v>
       </c>
@@ -4622,7 +4635,7 @@
         <v>9823000</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>312</v>
       </c>
@@ -4639,7 +4652,7 @@
         <v>336060</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>315</v>
       </c>
@@ -4656,7 +4669,7 @@
         <v>1298120000</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>318</v>
       </c>
@@ -4673,7 +4686,7 @@
         <v>260581000</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>321</v>
       </c>
@@ -4693,7 +4706,7 @@
         <v>79546600</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>325</v>
       </c>
@@ -4710,7 +4723,7 @@
         <v>37883543</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>328</v>
       </c>
@@ -4727,7 +4740,7 @@
         <v>4757976</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -4744,7 +4757,7 @@
         <v>84497</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -4761,7 +4774,7 @@
         <v>8584380</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -4778,7 +4791,7 @@
         <v>60665551</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -4795,7 +4808,7 @@
         <v>2723246</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>343</v>
       </c>
@@ -4812,7 +4825,7 @@
         <v>127000000</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>346</v>
       </c>
@@ -4829,7 +4842,7 @@
         <v>102700</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>349</v>
       </c>
@@ -4846,7 +4859,7 @@
         <v>9663560</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>352</v>
       </c>
@@ -4863,7 +4876,7 @@
         <v>17753200</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -4880,7 +4893,7 @@
         <v>47251000</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>358</v>
       </c>
@@ -4897,7 +4910,7 @@
         <v>113400</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -4917,7 +4930,7 @@
         <v>24213510</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>365</v>
       </c>
@@ -4937,7 +4950,7 @@
         <v>50617045</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>369</v>
       </c>
@@ -4954,7 +4967,7 @@
         <v>4183658</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>372</v>
       </c>
@@ -4971,7 +4984,7 @@
         <v>6047800</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>375</v>
       </c>
@@ -4991,7 +5004,7 @@
         <v>6492400</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>379</v>
       </c>
@@ -5008,7 +5021,7 @@
         <v>1958800</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>382</v>
       </c>
@@ -5025,7 +5038,7 @@
         <v>5988000</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>385</v>
       </c>
@@ -5042,7 +5055,7 @@
         <v>1916000</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>388</v>
       </c>
@@ -5059,7 +5072,7 @@
         <v>4076530</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>391</v>
       </c>
@@ -5076,7 +5089,7 @@
         <v>6385000</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>394</v>
       </c>
@@ -5093,7 +5106,7 @@
         <v>37623</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>397</v>
       </c>
@@ -5110,7 +5123,7 @@
         <v>2862786</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>400</v>
       </c>
@@ -5127,7 +5140,7 @@
         <v>576200</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>403</v>
       </c>
@@ -5144,7 +5157,7 @@
         <v>652500</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>406</v>
       </c>
@@ -5164,7 +5177,7 @@
         <v>2071278</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>410</v>
       </c>
@@ -5181,7 +5194,7 @@
         <v>22434363</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>413</v>
       </c>
@@ -5198,7 +5211,7 @@
         <v>16832910</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>416</v>
       </c>
@@ -5215,7 +5228,7 @@
         <v>31763200</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>419</v>
       </c>
@@ -5232,7 +5245,7 @@
         <v>344023</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>422</v>
       </c>
@@ -5249,7 +5262,7 @@
         <v>18341000</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>425</v>
       </c>
@@ -5266,7 +5279,7 @@
         <v>429344</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>428</v>
       </c>
@@ -5283,7 +5296,7 @@
         <v>54880</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>431</v>
       </c>
@@ -5300,7 +5313,7 @@
         <v>378243</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>434</v>
       </c>
@@ -5317,7 +5330,7 @@
         <v>3718678</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>437</v>
       </c>
@@ -5334,7 +5347,7 @@
         <v>1262879</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>440</v>
       </c>
@@ -5351,7 +5364,7 @@
         <v>226915</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>443</v>
       </c>
@@ -5368,7 +5381,7 @@
         <v>128632000</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>446</v>
       </c>
@@ -5385,7 +5398,7 @@
         <v>102800</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>449</v>
       </c>
@@ -5405,7 +5418,7 @@
         <v>3553100</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>453</v>
       </c>
@@ -5422,7 +5435,7 @@
         <v>38400</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>456</v>
       </c>
@@ -5439,7 +5452,7 @@
         <v>3105700</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>459</v>
       </c>
@@ -5456,7 +5469,7 @@
         <v>621810</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>462</v>
       </c>
@@ -5473,7 +5486,7 @@
         <v>4922</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>465</v>
       </c>
@@ -5490,7 +5503,7 @@
         <v>34086000</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>468</v>
       </c>
@@ -5507,7 +5520,7 @@
         <v>26423700</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>471</v>
       </c>
@@ -5524,15 +5537,15 @@
         <v>54363426</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>474</v>
       </c>
       <c r="B155" t="s">
+        <v>784</v>
+      </c>
+      <c r="C155" t="s">
         <v>475</v>
-      </c>
-      <c r="C155" t="s">
-        <v>476</v>
       </c>
       <c r="D155">
         <v>516</v>
@@ -5541,15 +5554,15 @@
         <v>2324388</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>476</v>
+      </c>
+      <c r="B156" t="s">
         <v>477</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" t="s">
         <v>478</v>
-      </c>
-      <c r="C156" t="s">
-        <v>479</v>
       </c>
       <c r="D156">
         <v>520</v>
@@ -5558,15 +5571,15 @@
         <v>10084</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>479</v>
+      </c>
+      <c r="B157" t="s">
         <v>480</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>481</v>
-      </c>
-      <c r="C157" t="s">
-        <v>482</v>
       </c>
       <c r="D157">
         <v>524</v>
@@ -5575,15 +5588,15 @@
         <v>28431500</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>482</v>
+      </c>
+      <c r="B158" t="s">
         <v>483</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>484</v>
-      </c>
-      <c r="C158" t="s">
-        <v>485</v>
       </c>
       <c r="D158">
         <v>528</v>
@@ -5592,15 +5605,15 @@
         <v>17050000</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>485</v>
+      </c>
+      <c r="B159" t="s">
         <v>486</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" t="s">
         <v>487</v>
-      </c>
-      <c r="C159" t="s">
-        <v>488</v>
       </c>
       <c r="D159">
         <v>540</v>
@@ -5609,15 +5622,15 @@
         <v>268767</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>488</v>
+      </c>
+      <c r="B160" t="s">
         <v>489</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
         <v>490</v>
-      </c>
-      <c r="C160" t="s">
-        <v>491</v>
       </c>
       <c r="D160">
         <v>554</v>
@@ -5626,15 +5639,15 @@
         <v>4716170</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>491</v>
+      </c>
+      <c r="B161" t="s">
         <v>492</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
         <v>493</v>
-      </c>
-      <c r="C161" t="s">
-        <v>494</v>
       </c>
       <c r="D161">
         <v>558</v>
@@ -5643,15 +5656,15 @@
         <v>6262703</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>494</v>
+      </c>
+      <c r="B162" t="s">
         <v>495</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>496</v>
-      </c>
-      <c r="C162" t="s">
-        <v>497</v>
       </c>
       <c r="D162">
         <v>562</v>
@@ -5660,15 +5673,15 @@
         <v>20715000</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>497</v>
+      </c>
+      <c r="B163" t="s">
         <v>498</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" t="s">
         <v>499</v>
-      </c>
-      <c r="C163" t="s">
-        <v>500</v>
       </c>
       <c r="D163">
         <v>566</v>
@@ -5677,15 +5690,15 @@
         <v>186988000</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>500</v>
+      </c>
+      <c r="B164" t="s">
         <v>501</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>502</v>
-      </c>
-      <c r="C164" t="s">
-        <v>503</v>
       </c>
       <c r="D164">
         <v>570</v>
@@ -5694,15 +5707,15 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>503</v>
+      </c>
+      <c r="B165" t="s">
         <v>504</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
         <v>505</v>
-      </c>
-      <c r="C165" t="s">
-        <v>506</v>
       </c>
       <c r="D165">
         <v>574</v>
@@ -5711,15 +5724,15 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>506</v>
+      </c>
+      <c r="B166" t="s">
         <v>507</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
         <v>508</v>
-      </c>
-      <c r="C166" t="s">
-        <v>509</v>
       </c>
       <c r="D166">
         <v>580</v>
@@ -5728,15 +5741,15 @@
         <v>56940</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>509</v>
+      </c>
+      <c r="B167" t="s">
         <v>510</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
         <v>511</v>
-      </c>
-      <c r="C167" t="s">
-        <v>512</v>
       </c>
       <c r="D167">
         <v>578</v>
@@ -5745,15 +5758,15 @@
         <v>5236826</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>512</v>
+      </c>
+      <c r="B168" t="s">
         <v>513</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>514</v>
-      </c>
-      <c r="C168" t="s">
-        <v>515</v>
       </c>
       <c r="D168">
         <v>512</v>
@@ -5762,15 +5775,15 @@
         <v>4496760</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>515</v>
+      </c>
+      <c r="B169" t="s">
         <v>516</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>517</v>
-      </c>
-      <c r="C169" t="s">
-        <v>518</v>
       </c>
       <c r="D169">
         <v>586</v>
@@ -5779,15 +5792,15 @@
         <v>194297000</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>518</v>
+      </c>
+      <c r="B170" t="s">
         <v>519</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>520</v>
-      </c>
-      <c r="C170" t="s">
-        <v>521</v>
       </c>
       <c r="D170">
         <v>585</v>
@@ -5796,35 +5809,35 @@
         <v>17950</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>521</v>
+      </c>
+      <c r="B171" t="s">
         <v>522</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
         <v>523</v>
-      </c>
-      <c r="C171" t="s">
-        <v>524</v>
       </c>
       <c r="D171">
         <v>275</v>
       </c>
       <c r="E171" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F171" s="2">
         <v>4816503</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>525</v>
+      </c>
+      <c r="B172" t="s">
         <v>526</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>527</v>
-      </c>
-      <c r="C172" t="s">
-        <v>528</v>
       </c>
       <c r="D172">
         <v>591</v>
@@ -5833,15 +5846,15 @@
         <v>3814672</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>528</v>
+      </c>
+      <c r="B173" t="s">
         <v>529</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
         <v>530</v>
-      </c>
-      <c r="C173" t="s">
-        <v>531</v>
       </c>
       <c r="D173">
         <v>598</v>
@@ -5850,15 +5863,15 @@
         <v>8083700</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>531</v>
+      </c>
+      <c r="B174" t="s">
         <v>532</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>533</v>
-      </c>
-      <c r="C174" t="s">
-        <v>534</v>
       </c>
       <c r="D174">
         <v>600</v>
@@ -5867,15 +5880,15 @@
         <v>6854536</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>534</v>
+      </c>
+      <c r="B175" t="s">
         <v>535</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
         <v>536</v>
-      </c>
-      <c r="C175" t="s">
-        <v>537</v>
       </c>
       <c r="D175">
         <v>604</v>
@@ -5884,15 +5897,15 @@
         <v>31488700</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>537</v>
+      </c>
+      <c r="B176" t="s">
         <v>538</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>539</v>
-      </c>
-      <c r="C176" t="s">
-        <v>540</v>
       </c>
       <c r="D176">
         <v>608</v>
@@ -5901,15 +5914,15 @@
         <v>103035000</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
+        <v>540</v>
+      </c>
+      <c r="B177" t="s">
         <v>541</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" t="s">
         <v>542</v>
-      </c>
-      <c r="C177" t="s">
-        <v>543</v>
       </c>
       <c r="D177">
         <v>612</v>
@@ -5918,15 +5931,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
+        <v>543</v>
+      </c>
+      <c r="B178" t="s">
         <v>544</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C178" t="s">
         <v>545</v>
-      </c>
-      <c r="C178" t="s">
-        <v>546</v>
       </c>
       <c r="D178">
         <v>616</v>
@@ -5935,15 +5948,15 @@
         <v>38437239</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>546</v>
+      </c>
+      <c r="B179" t="s">
         <v>547</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" t="s">
         <v>548</v>
-      </c>
-      <c r="C179" t="s">
-        <v>549</v>
       </c>
       <c r="D179">
         <v>620</v>
@@ -5952,15 +5965,15 @@
         <v>10341330</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>549</v>
+      </c>
+      <c r="B180" t="s">
         <v>550</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" t="s">
         <v>551</v>
-      </c>
-      <c r="C180" t="s">
-        <v>552</v>
       </c>
       <c r="D180">
         <v>630</v>
@@ -5969,15 +5982,15 @@
         <v>3474182</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>552</v>
+      </c>
+      <c r="B181" t="s">
         <v>553</v>
       </c>
-      <c r="B181" t="s">
+      <c r="C181" t="s">
         <v>554</v>
-      </c>
-      <c r="C181" t="s">
-        <v>555</v>
       </c>
       <c r="D181">
         <v>634</v>
@@ -5986,15 +5999,15 @@
         <v>2401598</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>555</v>
+      </c>
+      <c r="B182" t="s">
         <v>556</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>557</v>
-      </c>
-      <c r="C182" t="s">
-        <v>558</v>
       </c>
       <c r="D182">
         <v>638</v>
@@ -6003,15 +6016,15 @@
         <v>843529</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>558</v>
+      </c>
+      <c r="B183" t="s">
         <v>559</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C183" t="s">
         <v>560</v>
-      </c>
-      <c r="C183" t="s">
-        <v>561</v>
       </c>
       <c r="D183">
         <v>642</v>
@@ -6020,35 +6033,35 @@
         <v>19760000</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>561</v>
+      </c>
+      <c r="B184" t="s">
         <v>562</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>563</v>
-      </c>
-      <c r="C184" t="s">
-        <v>564</v>
       </c>
       <c r="D184">
         <v>643</v>
       </c>
       <c r="E184" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F184" s="2">
         <v>146654366</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>565</v>
+      </c>
+      <c r="B185" t="s">
         <v>566</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>567</v>
-      </c>
-      <c r="C185" t="s">
-        <v>568</v>
       </c>
       <c r="D185">
         <v>646</v>
@@ -6057,15 +6070,15 @@
         <v>11553188</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B186" t="s">
+        <v>568</v>
+      </c>
+      <c r="C186" t="s">
         <v>569</v>
-      </c>
-      <c r="C186" t="s">
-        <v>570</v>
       </c>
       <c r="D186">
         <v>652</v>
@@ -6074,35 +6087,35 @@
         <v>9417</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>570</v>
+      </c>
+      <c r="B187" t="s">
         <v>571</v>
       </c>
-      <c r="B187" t="s">
+      <c r="C187" t="s">
         <v>572</v>
-      </c>
-      <c r="C187" t="s">
-        <v>573</v>
       </c>
       <c r="D187">
         <v>654</v>
       </c>
       <c r="E187" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F187" s="2">
         <v>4255</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>574</v>
+      </c>
+      <c r="B188" t="s">
         <v>575</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
         <v>576</v>
-      </c>
-      <c r="C188" t="s">
-        <v>577</v>
       </c>
       <c r="D188">
         <v>659</v>
@@ -6111,15 +6124,15 @@
         <v>46204</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>577</v>
+      </c>
+      <c r="B189" t="s">
         <v>578</v>
       </c>
-      <c r="B189" t="s">
+      <c r="C189" t="s">
         <v>579</v>
-      </c>
-      <c r="C189" t="s">
-        <v>580</v>
       </c>
       <c r="D189">
         <v>662</v>
@@ -6128,15 +6141,15 @@
         <v>186000</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
+        <v>580</v>
+      </c>
+      <c r="B190" t="s">
         <v>581</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" t="s">
         <v>582</v>
-      </c>
-      <c r="C190" t="s">
-        <v>583</v>
       </c>
       <c r="D190">
         <v>663</v>
@@ -6145,15 +6158,15 @@
         <v>36457</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
+        <v>583</v>
+      </c>
+      <c r="B191" t="s">
         <v>584</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
         <v>585</v>
-      </c>
-      <c r="C191" t="s">
-        <v>586</v>
       </c>
       <c r="D191">
         <v>666</v>
@@ -6162,15 +6175,15 @@
         <v>6286</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>586</v>
+      </c>
+      <c r="B192" t="s">
         <v>587</v>
       </c>
-      <c r="B192" t="s">
+      <c r="C192" t="s">
         <v>588</v>
-      </c>
-      <c r="C192" t="s">
-        <v>589</v>
       </c>
       <c r="D192">
         <v>670</v>
@@ -6179,15 +6192,15 @@
         <v>109991</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>589</v>
+      </c>
+      <c r="B193" t="s">
         <v>590</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
         <v>591</v>
-      </c>
-      <c r="C193" t="s">
-        <v>592</v>
       </c>
       <c r="D193">
         <v>882</v>
@@ -6196,15 +6209,15 @@
         <v>194899</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>592</v>
+      </c>
+      <c r="B194" t="s">
         <v>593</v>
       </c>
-      <c r="B194" t="s">
+      <c r="C194" t="s">
         <v>594</v>
-      </c>
-      <c r="C194" t="s">
-        <v>595</v>
       </c>
       <c r="D194">
         <v>674</v>
@@ -6213,15 +6226,15 @@
         <v>33005</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>595</v>
+      </c>
+      <c r="B195" t="s">
         <v>596</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195" t="s">
         <v>597</v>
-      </c>
-      <c r="C195" t="s">
-        <v>598</v>
       </c>
       <c r="D195">
         <v>678</v>
@@ -6230,15 +6243,15 @@
         <v>187356</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>598</v>
+      </c>
+      <c r="B196" t="s">
         <v>599</v>
       </c>
-      <c r="B196" t="s">
+      <c r="C196" t="s">
         <v>600</v>
-      </c>
-      <c r="C196" t="s">
-        <v>601</v>
       </c>
       <c r="D196">
         <v>682</v>
@@ -6247,15 +6260,15 @@
         <v>31015999</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>601</v>
+      </c>
+      <c r="B197" t="s">
         <v>602</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>603</v>
-      </c>
-      <c r="C197" t="s">
-        <v>604</v>
       </c>
       <c r="D197">
         <v>686</v>
@@ -6264,15 +6277,15 @@
         <v>14799859</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>604</v>
+      </c>
+      <c r="B198" t="s">
         <v>605</v>
       </c>
-      <c r="B198" t="s">
+      <c r="C198" t="s">
         <v>606</v>
-      </c>
-      <c r="C198" t="s">
-        <v>607</v>
       </c>
       <c r="D198">
         <v>688</v>
@@ -6281,15 +6294,15 @@
         <v>7076372</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
+        <v>607</v>
+      </c>
+      <c r="B199" t="s">
         <v>608</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>609</v>
-      </c>
-      <c r="C199" t="s">
-        <v>610</v>
       </c>
       <c r="D199">
         <v>690</v>
@@ -6298,15 +6311,15 @@
         <v>93144</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>610</v>
+      </c>
+      <c r="B200" t="s">
         <v>611</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
         <v>612</v>
-      </c>
-      <c r="C200" t="s">
-        <v>613</v>
       </c>
       <c r="D200">
         <v>694</v>
@@ -6315,15 +6328,15 @@
         <v>7075641</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>613</v>
+      </c>
+      <c r="B201" t="s">
         <v>614</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
         <v>615</v>
-      </c>
-      <c r="C201" t="s">
-        <v>616</v>
       </c>
       <c r="D201">
         <v>702</v>
@@ -6332,15 +6345,15 @@
         <v>5535000</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>616</v>
+      </c>
+      <c r="B202" t="s">
         <v>617</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>618</v>
-      </c>
-      <c r="C202" t="s">
-        <v>619</v>
       </c>
       <c r="D202">
         <v>534</v>
@@ -6349,15 +6362,15 @@
         <v>38247</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>619</v>
+      </c>
+      <c r="B203" t="s">
         <v>620</v>
       </c>
-      <c r="B203" t="s">
+      <c r="C203" t="s">
         <v>621</v>
-      </c>
-      <c r="C203" t="s">
-        <v>622</v>
       </c>
       <c r="D203">
         <v>703</v>
@@ -6366,15 +6379,15 @@
         <v>5426252</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>622</v>
+      </c>
+      <c r="B204" t="s">
         <v>623</v>
       </c>
-      <c r="B204" t="s">
+      <c r="C204" t="s">
         <v>624</v>
-      </c>
-      <c r="C204" t="s">
-        <v>625</v>
       </c>
       <c r="D204">
         <v>705</v>
@@ -6383,15 +6396,15 @@
         <v>2063371</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>625</v>
+      </c>
+      <c r="B205" t="s">
         <v>626</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>627</v>
-      </c>
-      <c r="C205" t="s">
-        <v>628</v>
       </c>
       <c r="D205">
         <v>90</v>
@@ -6400,15 +6413,15 @@
         <v>642000</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>628</v>
+      </c>
+      <c r="B206" t="s">
         <v>629</v>
       </c>
-      <c r="B206" t="s">
+      <c r="C206" t="s">
         <v>630</v>
-      </c>
-      <c r="C206" t="s">
-        <v>631</v>
       </c>
       <c r="D206">
         <v>706</v>
@@ -6417,15 +6430,15 @@
         <v>11079000</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
+        <v>631</v>
+      </c>
+      <c r="B207" t="s">
         <v>632</v>
       </c>
-      <c r="B207" t="s">
+      <c r="C207" t="s">
         <v>633</v>
-      </c>
-      <c r="C207" t="s">
-        <v>634</v>
       </c>
       <c r="D207">
         <v>710</v>
@@ -6434,15 +6447,15 @@
         <v>55653654</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>634</v>
+      </c>
+      <c r="B208" t="s">
         <v>635</v>
       </c>
-      <c r="B208" t="s">
+      <c r="C208" t="s">
         <v>636</v>
-      </c>
-      <c r="C208" t="s">
-        <v>637</v>
       </c>
       <c r="D208">
         <v>239</v>
@@ -6451,15 +6464,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>637</v>
+      </c>
+      <c r="B209" t="s">
         <v>638</v>
       </c>
-      <c r="B209" t="s">
+      <c r="C209" t="s">
         <v>639</v>
-      </c>
-      <c r="C209" t="s">
-        <v>640</v>
       </c>
       <c r="D209">
         <v>728</v>
@@ -6468,15 +6481,15 @@
         <v>12131000</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
+        <v>640</v>
+      </c>
+      <c r="B210" t="s">
         <v>641</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>642</v>
-      </c>
-      <c r="C210" t="s">
-        <v>643</v>
       </c>
       <c r="D210">
         <v>724</v>
@@ -6485,15 +6498,15 @@
         <v>46438422</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>643</v>
+      </c>
+      <c r="B211" t="s">
         <v>644</v>
       </c>
-      <c r="B211" t="s">
+      <c r="C211" t="s">
         <v>645</v>
-      </c>
-      <c r="C211" t="s">
-        <v>646</v>
       </c>
       <c r="D211">
         <v>144</v>
@@ -6502,15 +6515,15 @@
         <v>20966000</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>646</v>
+      </c>
+      <c r="B212" t="s">
         <v>647</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>648</v>
-      </c>
-      <c r="C212" t="s">
-        <v>649</v>
       </c>
       <c r="D212">
         <v>729</v>
@@ -6519,15 +6532,15 @@
         <v>41176000</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>649</v>
+      </c>
+      <c r="B213" t="s">
         <v>650</v>
       </c>
-      <c r="B213" t="s">
+      <c r="C213" t="s">
         <v>651</v>
-      </c>
-      <c r="C213" t="s">
-        <v>652</v>
       </c>
       <c r="D213">
         <v>740</v>
@@ -6536,15 +6549,15 @@
         <v>541638</v>
       </c>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
+        <v>652</v>
+      </c>
+      <c r="B214" t="s">
         <v>653</v>
       </c>
-      <c r="B214" t="s">
+      <c r="C214" t="s">
         <v>654</v>
-      </c>
-      <c r="C214" t="s">
-        <v>655</v>
       </c>
       <c r="D214">
         <v>744</v>
@@ -6553,15 +6566,15 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
+        <v>655</v>
+      </c>
+      <c r="B215" t="s">
         <v>656</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
         <v>657</v>
-      </c>
-      <c r="C215" t="s">
-        <v>658</v>
       </c>
       <c r="D215">
         <v>748</v>
@@ -6570,15 +6583,15 @@
         <v>1132657</v>
       </c>
     </row>
-    <row r="216" spans="1:6">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>658</v>
+      </c>
+      <c r="B216" t="s">
         <v>659</v>
       </c>
-      <c r="B216" t="s">
+      <c r="C216" t="s">
         <v>660</v>
-      </c>
-      <c r="C216" t="s">
-        <v>661</v>
       </c>
       <c r="D216">
         <v>752</v>
@@ -6587,15 +6600,15 @@
         <v>9920881</v>
       </c>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
+        <v>661</v>
+      </c>
+      <c r="B217" t="s">
         <v>662</v>
       </c>
-      <c r="B217" t="s">
+      <c r="C217" t="s">
         <v>663</v>
-      </c>
-      <c r="C217" t="s">
-        <v>664</v>
       </c>
       <c r="D217">
         <v>756</v>
@@ -6604,35 +6617,35 @@
         <v>8341600</v>
       </c>
     </row>
-    <row r="218" spans="1:6">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
+        <v>664</v>
+      </c>
+      <c r="B218" t="s">
         <v>665</v>
       </c>
-      <c r="B218" t="s">
+      <c r="C218" t="s">
         <v>666</v>
-      </c>
-      <c r="C218" t="s">
-        <v>667</v>
       </c>
       <c r="D218">
         <v>760</v>
       </c>
       <c r="E218" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F218" s="2">
         <v>18564000</v>
       </c>
     </row>
-    <row r="219" spans="1:6">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
+        <v>668</v>
+      </c>
+      <c r="B219" t="s">
         <v>669</v>
       </c>
-      <c r="B219" t="s">
+      <c r="C219" t="s">
         <v>670</v>
-      </c>
-      <c r="C219" t="s">
-        <v>671</v>
       </c>
       <c r="D219">
         <v>158</v>
@@ -6641,15 +6654,15 @@
         <v>23514750</v>
       </c>
     </row>
-    <row r="220" spans="1:6">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>671</v>
+      </c>
+      <c r="B220" t="s">
         <v>672</v>
       </c>
-      <c r="B220" t="s">
+      <c r="C220" t="s">
         <v>673</v>
-      </c>
-      <c r="C220" t="s">
-        <v>674</v>
       </c>
       <c r="D220">
         <v>762</v>
@@ -6658,35 +6671,35 @@
         <v>8551000</v>
       </c>
     </row>
-    <row r="221" spans="1:6">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>674</v>
+      </c>
+      <c r="B221" t="s">
         <v>675</v>
       </c>
-      <c r="B221" t="s">
+      <c r="C221" t="s">
         <v>676</v>
-      </c>
-      <c r="C221" t="s">
-        <v>677</v>
       </c>
       <c r="D221">
         <v>834</v>
       </c>
       <c r="E221" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F221" s="2">
         <v>55155000</v>
       </c>
     </row>
-    <row r="222" spans="1:6">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>678</v>
+      </c>
+      <c r="B222" t="s">
         <v>679</v>
       </c>
-      <c r="B222" t="s">
+      <c r="C222" t="s">
         <v>680</v>
-      </c>
-      <c r="C222" t="s">
-        <v>681</v>
       </c>
       <c r="D222">
         <v>764</v>
@@ -6695,15 +6708,15 @@
         <v>65729098</v>
       </c>
     </row>
-    <row r="223" spans="1:6">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
+        <v>681</v>
+      </c>
+      <c r="B223" t="s">
         <v>682</v>
       </c>
-      <c r="B223" t="s">
+      <c r="C223" t="s">
         <v>683</v>
-      </c>
-      <c r="C223" t="s">
-        <v>684</v>
       </c>
       <c r="D223">
         <v>626</v>
@@ -6712,15 +6725,15 @@
         <v>1167242</v>
       </c>
     </row>
-    <row r="224" spans="1:6">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
+        <v>684</v>
+      </c>
+      <c r="B224" t="s">
         <v>685</v>
       </c>
-      <c r="B224" t="s">
+      <c r="C224" t="s">
         <v>686</v>
-      </c>
-      <c r="C224" t="s">
-        <v>687</v>
       </c>
       <c r="D224">
         <v>768</v>
@@ -6729,15 +6742,15 @@
         <v>7143000</v>
       </c>
     </row>
-    <row r="225" spans="1:6">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>687</v>
+      </c>
+      <c r="B225" t="s">
         <v>688</v>
       </c>
-      <c r="B225" t="s">
+      <c r="C225" t="s">
         <v>689</v>
-      </c>
-      <c r="C225" t="s">
-        <v>690</v>
       </c>
       <c r="D225">
         <v>772</v>
@@ -6746,15 +6759,15 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
+        <v>690</v>
+      </c>
+      <c r="B226" t="s">
         <v>691</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
         <v>692</v>
-      </c>
-      <c r="C226" t="s">
-        <v>693</v>
       </c>
       <c r="D226">
         <v>776</v>
@@ -6763,15 +6776,15 @@
         <v>103252</v>
       </c>
     </row>
-    <row r="227" spans="1:6">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
+        <v>693</v>
+      </c>
+      <c r="B227" t="s">
         <v>694</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
         <v>695</v>
-      </c>
-      <c r="C227" t="s">
-        <v>696</v>
       </c>
       <c r="D227">
         <v>780</v>
@@ -6780,15 +6793,15 @@
         <v>1349667</v>
       </c>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
+        <v>696</v>
+      </c>
+      <c r="B228" t="s">
         <v>697</v>
       </c>
-      <c r="B228" t="s">
+      <c r="C228" t="s">
         <v>698</v>
-      </c>
-      <c r="C228" t="s">
-        <v>699</v>
       </c>
       <c r="D228">
         <v>788</v>
@@ -6797,15 +6810,15 @@
         <v>11154400</v>
       </c>
     </row>
-    <row r="229" spans="1:6">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
+        <v>699</v>
+      </c>
+      <c r="B229" t="s">
         <v>700</v>
       </c>
-      <c r="B229" t="s">
+      <c r="C229" t="s">
         <v>701</v>
-      </c>
-      <c r="C229" t="s">
-        <v>702</v>
       </c>
       <c r="D229">
         <v>792</v>
@@ -6814,15 +6827,15 @@
         <v>78742000</v>
       </c>
     </row>
-    <row r="230" spans="1:6">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
+        <v>702</v>
+      </c>
+      <c r="B230" t="s">
         <v>703</v>
       </c>
-      <c r="B230" t="s">
+      <c r="C230" t="s">
         <v>704</v>
-      </c>
-      <c r="C230" t="s">
-        <v>705</v>
       </c>
       <c r="D230">
         <v>795</v>
@@ -6831,15 +6844,15 @@
         <v>4751120</v>
       </c>
     </row>
-    <row r="231" spans="1:6">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
+        <v>705</v>
+      </c>
+      <c r="B231" t="s">
         <v>706</v>
       </c>
-      <c r="B231" t="s">
+      <c r="C231" t="s">
         <v>707</v>
-      </c>
-      <c r="C231" t="s">
-        <v>708</v>
       </c>
       <c r="D231">
         <v>796</v>
@@ -6848,15 +6861,15 @@
         <v>31458</v>
       </c>
     </row>
-    <row r="232" spans="1:6">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>708</v>
+      </c>
+      <c r="B232" t="s">
         <v>709</v>
       </c>
-      <c r="B232" t="s">
+      <c r="C232" t="s">
         <v>710</v>
-      </c>
-      <c r="C232" t="s">
-        <v>711</v>
       </c>
       <c r="D232">
         <v>798</v>
@@ -6865,15 +6878,15 @@
         <v>10640</v>
       </c>
     </row>
-    <row r="233" spans="1:6">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
+        <v>711</v>
+      </c>
+      <c r="B233" t="s">
         <v>712</v>
       </c>
-      <c r="B233" t="s">
+      <c r="C233" t="s">
         <v>713</v>
-      </c>
-      <c r="C233" t="s">
-        <v>714</v>
       </c>
       <c r="D233">
         <v>800</v>
@@ -6882,15 +6895,15 @@
         <v>36861000</v>
       </c>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
+        <v>714</v>
+      </c>
+      <c r="B234" t="s">
         <v>715</v>
       </c>
-      <c r="B234" t="s">
+      <c r="C234" t="s">
         <v>716</v>
-      </c>
-      <c r="C234" t="s">
-        <v>717</v>
       </c>
       <c r="D234">
         <v>804</v>
@@ -6899,15 +6912,15 @@
         <v>42658149</v>
       </c>
     </row>
-    <row r="235" spans="1:6">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
+        <v>717</v>
+      </c>
+      <c r="B235" t="s">
         <v>718</v>
       </c>
-      <c r="B235" t="s">
+      <c r="C235" t="s">
         <v>719</v>
-      </c>
-      <c r="C235" t="s">
-        <v>720</v>
       </c>
       <c r="D235">
         <v>784</v>
@@ -6916,15 +6929,15 @@
         <v>9856000</v>
       </c>
     </row>
-    <row r="236" spans="1:6">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
+        <v>720</v>
+      </c>
+      <c r="B236" t="s">
         <v>721</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
         <v>722</v>
-      </c>
-      <c r="C236" t="s">
-        <v>723</v>
       </c>
       <c r="D236">
         <v>826</v>
@@ -6933,15 +6946,15 @@
         <v>65110000</v>
       </c>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
+        <v>723</v>
+      </c>
+      <c r="B237" t="s">
         <v>724</v>
       </c>
-      <c r="B237" t="s">
+      <c r="C237" t="s">
         <v>725</v>
-      </c>
-      <c r="C237" t="s">
-        <v>726</v>
       </c>
       <c r="D237">
         <v>840</v>
@@ -6950,15 +6963,15 @@
         <v>324515000</v>
       </c>
     </row>
-    <row r="238" spans="1:6">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>726</v>
+      </c>
+      <c r="B238" t="s">
         <v>727</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>728</v>
-      </c>
-      <c r="C238" t="s">
-        <v>729</v>
       </c>
       <c r="D238">
         <v>581</v>
@@ -6967,15 +6980,15 @@
         <v>300</v>
       </c>
     </row>
-    <row r="239" spans="1:6">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
+        <v>729</v>
+      </c>
+      <c r="B239" t="s">
         <v>730</v>
       </c>
-      <c r="B239" t="s">
+      <c r="C239" t="s">
         <v>731</v>
-      </c>
-      <c r="C239" t="s">
-        <v>732</v>
       </c>
       <c r="D239">
         <v>858</v>
@@ -6984,15 +6997,15 @@
         <v>3480222</v>
       </c>
     </row>
-    <row r="240" spans="1:6">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>732</v>
+      </c>
+      <c r="B240" t="s">
         <v>733</v>
       </c>
-      <c r="B240" t="s">
+      <c r="C240" t="s">
         <v>734</v>
-      </c>
-      <c r="C240" t="s">
-        <v>735</v>
       </c>
       <c r="D240">
         <v>860</v>
@@ -7001,15 +7014,15 @@
         <v>31575300</v>
       </c>
     </row>
-    <row r="241" spans="1:6">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
+        <v>735</v>
+      </c>
+      <c r="B241" t="s">
         <v>736</v>
       </c>
-      <c r="B241" t="s">
+      <c r="C241" t="s">
         <v>737</v>
-      </c>
-      <c r="C241" t="s">
-        <v>738</v>
       </c>
       <c r="D241">
         <v>548</v>
@@ -7018,35 +7031,35 @@
         <v>277500</v>
       </c>
     </row>
-    <row r="242" spans="1:6">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
+        <v>738</v>
+      </c>
+      <c r="B242" t="s">
         <v>739</v>
       </c>
-      <c r="B242" t="s">
+      <c r="C242" t="s">
         <v>740</v>
-      </c>
-      <c r="C242" t="s">
-        <v>741</v>
       </c>
       <c r="D242">
         <v>862</v>
       </c>
       <c r="E242" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F242" s="2">
         <v>31028700</v>
       </c>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>742</v>
+      </c>
+      <c r="B243" t="s">
         <v>743</v>
       </c>
-      <c r="B243" t="s">
+      <c r="C243" t="s">
         <v>744</v>
-      </c>
-      <c r="C243" t="s">
-        <v>745</v>
       </c>
       <c r="D243">
         <v>704</v>
@@ -7055,15 +7068,15 @@
         <v>92700000</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
+        <v>745</v>
+      </c>
+      <c r="B244" t="s">
         <v>746</v>
       </c>
-      <c r="B244" t="s">
+      <c r="C244" t="s">
         <v>747</v>
-      </c>
-      <c r="C244" t="s">
-        <v>748</v>
       </c>
       <c r="D244">
         <v>92</v>
@@ -7072,15 +7085,15 @@
         <v>28514</v>
       </c>
     </row>
-    <row r="245" spans="1:6">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
+        <v>748</v>
+      </c>
+      <c r="B245" t="s">
         <v>749</v>
       </c>
-      <c r="B245" t="s">
+      <c r="C245" t="s">
         <v>750</v>
-      </c>
-      <c r="C245" t="s">
-        <v>751</v>
       </c>
       <c r="D245">
         <v>850</v>
@@ -7089,15 +7102,15 @@
         <v>106000</v>
       </c>
     </row>
-    <row r="246" spans="1:6">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
+        <v>751</v>
+      </c>
+      <c r="B246" t="s">
         <v>752</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C246" t="s">
         <v>753</v>
-      </c>
-      <c r="C246" t="s">
-        <v>754</v>
       </c>
       <c r="D246">
         <v>876</v>
@@ -7106,15 +7119,15 @@
         <v>11750</v>
       </c>
     </row>
-    <row r="247" spans="1:6">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
+        <v>754</v>
+      </c>
+      <c r="B247" t="s">
         <v>755</v>
       </c>
-      <c r="B247" t="s">
+      <c r="C247" t="s">
         <v>756</v>
-      </c>
-      <c r="C247" t="s">
-        <v>757</v>
       </c>
       <c r="D247">
         <v>732</v>
@@ -7123,15 +7136,15 @@
         <v>584000</v>
       </c>
     </row>
-    <row r="248" spans="1:6">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
+        <v>757</v>
+      </c>
+      <c r="B248" t="s">
         <v>758</v>
       </c>
-      <c r="B248" t="s">
+      <c r="C248" t="s">
         <v>759</v>
-      </c>
-      <c r="C248" t="s">
-        <v>760</v>
       </c>
       <c r="D248">
         <v>887</v>
@@ -7140,15 +7153,15 @@
         <v>27478000</v>
       </c>
     </row>
-    <row r="249" spans="1:6">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
+        <v>760</v>
+      </c>
+      <c r="B249" t="s">
         <v>761</v>
       </c>
-      <c r="B249" t="s">
+      <c r="C249" t="s">
         <v>762</v>
-      </c>
-      <c r="C249" t="s">
-        <v>763</v>
       </c>
       <c r="D249">
         <v>894</v>
@@ -7157,15 +7170,15 @@
         <v>15933883</v>
       </c>
     </row>
-    <row r="250" spans="1:6">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
+        <v>763</v>
+      </c>
+      <c r="B250" t="s">
         <v>764</v>
       </c>
-      <c r="B250" t="s">
+      <c r="C250" t="s">
         <v>765</v>
-      </c>
-      <c r="C250" t="s">
-        <v>766</v>
       </c>
       <c r="D250">
         <v>716</v>
@@ -7174,72 +7187,72 @@
         <v>14240168</v>
       </c>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
+        <v>766</v>
+      </c>
+      <c r="B251" t="s">
         <v>767</v>
       </c>
-      <c r="B251" t="s">
+      <c r="C251" t="s">
         <v>768</v>
-      </c>
-      <c r="C251" t="s">
-        <v>769</v>
       </c>
       <c r="D251">
         <v>902</v>
       </c>
       <c r="E251" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="252" spans="1:6">
-      <c r="A252" t="s">
+      <c r="B252" t="s">
         <v>771</v>
       </c>
-      <c r="B252" t="s">
+      <c r="C252" t="s">
         <v>772</v>
-      </c>
-      <c r="C252" t="s">
-        <v>773</v>
       </c>
       <c r="D252">
         <v>903</v>
       </c>
       <c r="E252" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="253" spans="1:6">
-      <c r="A253" t="s">
+      <c r="B253" t="s">
         <v>775</v>
       </c>
-      <c r="B253" t="s">
+      <c r="C253" t="s">
         <v>776</v>
-      </c>
-      <c r="C253" t="s">
-        <v>777</v>
       </c>
       <c r="D253">
         <v>904</v>
       </c>
       <c r="E253" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="254" spans="1:6">
-      <c r="A254" t="s">
+      <c r="B254" t="s">
         <v>779</v>
       </c>
-      <c r="B254" t="s">
+      <c r="C254" t="s">
         <v>780</v>
-      </c>
-      <c r="C254" t="s">
-        <v>781</v>
       </c>
       <c r="D254">
         <v>0</v>
       </c>
       <c r="E254" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F254" s="2">
         <v>0</v>
@@ -7248,10 +7261,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>